<commit_message>
Added pyrite, 50 Bq FHY pH9
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -2646,7 +2646,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,16 +3432,23 @@
       <c r="B33" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="C33" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D33" s="21">
+        <f>C33*3.8/100</f>
+        <v>2.2040000000000002E-3</v>
+      </c>
       <c r="E33" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F33" s="1">
         <f>(C33-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>-4.9863554343643806</v>
+        <v>39.146000743058828</v>
       </c>
       <c r="G33" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F33-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>74.035276446395159</v>
+        <v>567.79850308782375</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3451,16 +3458,23 @@
       <c r="B34" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="C34" s="21">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D34" s="21">
+        <f>3.2/100*C34</f>
+        <v>1.8240000000000001E-3</v>
+      </c>
       <c r="E34" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F34" s="1">
         <f>(C34-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>-4.9863554343643806</v>
+        <v>38.385098050344638</v>
       </c>
       <c r="G34" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F34-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>74.035276446395159</v>
+        <v>556.73647081686329</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3470,16 +3484,23 @@
       <c r="B35" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="C35" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D35" s="21">
+        <f>3.6/100*C35</f>
+        <v>2.0880000000000004E-3</v>
+      </c>
       <c r="E35" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F35" s="1">
         <f>(C35-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>-4.9863554343643806</v>
+        <v>39.146000743058828</v>
       </c>
       <c r="G35" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F35-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>74.035276446395159</v>
+        <v>567.79850308782375</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -5566,10 +5587,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6494,262 +6515,283 @@
         <v>0.64413205376649052</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="33">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="33">
         <v>2E-3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="33">
         <v>8.94</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="34">
         <v>0.03</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="35">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="34">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="34">
         <v>5</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11">
+      <c r="I11" s="34">
+        <f>'Count-&gt;Actual Activity'!F11</f>
+        <v>0.25716654128242811</v>
+      </c>
+      <c r="J11" s="34"/>
+      <c r="K11" s="33">
         <v>10</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="33">
         <v>0.02</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="34">
         <f>'Count-&gt;Actual Activity'!F33</f>
-        <v>-4.9863554343643806</v>
-      </c>
-      <c r="N11" s="1">
+        <v>39.146000743058828</v>
+      </c>
+      <c r="N11" s="34">
         <f>'Count-&gt;Actual Activity'!G33</f>
-        <v>74.035276446395159</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11">
+        <v>567.79850308782375</v>
+      </c>
+      <c r="O11" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="P11" s="33">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="Q11" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R11" t="e">
+        <v>2.5716654128242811E-2</v>
+      </c>
+      <c r="R11" s="33">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S11" t="e">
+        <v>5.1433308256485625E-5</v>
+      </c>
+      <c r="S11" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T11" t="e">
+        <v>1304.8666914352943</v>
+      </c>
+      <c r="T11" s="33">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U11">
+        <v>18926.75171217525</v>
+      </c>
+      <c r="U11" s="33">
         <f>Parameters!$B$6*'Bottle Results'!B11</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="33">
         <f>SQRT((C11/B11)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X11">
+      <c r="W11" s="33">
+        <f t="shared" ref="W11:W19" si="7">(U11-S11*O11)/G11</f>
+        <v>0.1080742570015753</v>
+      </c>
+      <c r="X11" s="33">
         <v>2.3297919246001962E-2</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="33">
         <f t="shared" si="5"/>
-        <v>1665.1142147738788</v>
-      </c>
-      <c r="AA11" s="38" t="s">
+        <v>1579.3920343464026</v>
+      </c>
+      <c r="AA11" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="AB11">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="AB11" s="33">
+        <f>S11*E11/U11</f>
+        <v>0.78364996218141969</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="33">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="33">
         <v>2E-3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="33">
         <v>8.89</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="34">
         <v>0.03</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="35">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="34">
         <v>100</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="34">
         <v>5</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12">
+      <c r="I12" s="34">
+        <f>'Count-&gt;Actual Activity'!F12</f>
+        <v>0.25363929010379288</v>
+      </c>
+      <c r="J12" s="34"/>
+      <c r="K12" s="33">
         <v>10</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="33">
         <v>0.02</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="34">
         <f>'Count-&gt;Actual Activity'!F34</f>
-        <v>-4.9863554343643806</v>
-      </c>
-      <c r="N12" s="1">
+        <v>38.385098050344638</v>
+      </c>
+      <c r="N12" s="34">
         <f>'Count-&gt;Actual Activity'!G34</f>
-        <v>74.035276446395159</v>
-      </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12">
+        <v>556.73647081686329</v>
+      </c>
+      <c r="O12" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="P12" s="33">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="Q12" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R12" t="e">
+        <v>2.5363929010379288E-2</v>
+      </c>
+      <c r="R12" s="33">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S12" t="e">
+        <v>5.072785802075858E-5</v>
+      </c>
+      <c r="S12" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T12" t="e">
+        <v>1279.5032683448212</v>
+      </c>
+      <c r="T12" s="33">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U12">
+        <v>18558.014686229326</v>
+      </c>
+      <c r="U12" s="33">
         <f>Parameters!$B$6*'Bottle Results'!B12</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="33">
         <f>SQRT((C12/B12)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X12">
+      <c r="W12" s="33">
+        <f t="shared" si="7"/>
+        <v>0.1156832839287172</v>
+      </c>
+      <c r="X12" s="33">
         <v>2.3297917690924E-2</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="33">
         <f t="shared" si="5"/>
-        <v>1665.1142147738788</v>
-      </c>
-      <c r="AA12" s="38" t="s">
+        <v>1580.567784739281</v>
+      </c>
+      <c r="AA12" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="AB12">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="AB12" s="33">
+        <f>S12*E12/U12</f>
+        <v>0.76841771993315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="33">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="33">
         <v>2E-3</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="33">
         <v>8.92</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="34">
         <v>0.03</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="35">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="34">
         <v>100</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="34">
         <v>5</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13">
+      <c r="I13" s="34">
+        <f>'Count-&gt;Actual Activity'!F13</f>
+        <v>0.25911261089822724</v>
+      </c>
+      <c r="J13" s="34"/>
+      <c r="K13" s="33">
         <v>10</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="33">
         <v>0.02</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="34">
         <f>'Count-&gt;Actual Activity'!F35</f>
-        <v>-4.9863554343643806</v>
-      </c>
-      <c r="N13" s="1">
+        <v>39.146000743058828</v>
+      </c>
+      <c r="N13" s="34">
         <f>'Count-&gt;Actual Activity'!G35</f>
-        <v>74.035276446395159</v>
-      </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13">
+        <v>567.79850308782375</v>
+      </c>
+      <c r="O13" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="P13" s="33">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="Q13" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R13" t="e">
+        <v>2.5911261089822724E-2</v>
+      </c>
+      <c r="R13" s="33">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" t="e">
+        <v>5.182252217964545E-5</v>
+      </c>
+      <c r="S13" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T13" t="e">
+        <v>1304.8666914352943</v>
+      </c>
+      <c r="T13" s="33">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13">
+        <v>18926.75171217525</v>
+      </c>
+      <c r="U13" s="33">
         <f>Parameters!$B$6*'Bottle Results'!B13</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="33">
         <f>SQRT((C13/B13)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X13">
+      <c r="W13" s="33">
+        <f t="shared" si="7"/>
+        <v>0.1080742570015753</v>
+      </c>
+      <c r="X13" s="33">
         <v>2.3297920113197729E-2</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="33">
         <f t="shared" si="5"/>
-        <v>1665.1142147738788</v>
-      </c>
-      <c r="AA13" s="38" t="s">
+        <v>1578.7433444744695</v>
+      </c>
+      <c r="AA13" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="AB13">
-        <f t="shared" si="6"/>
-        <v>1</v>
+      <c r="AB13" s="33">
+        <f>S13*E13/U13</f>
+        <v>0.78364996218141969</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -6828,7 +6870,7 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W14" s="33">
-        <f>(U14-S14*O14)/G14</f>
+        <f t="shared" si="7"/>
         <v>0.21067607630596855</v>
       </c>
       <c r="X14" s="33">
@@ -6872,7 +6914,10 @@
       <c r="H15" s="34">
         <v>5</v>
       </c>
-      <c r="I15" s="34"/>
+      <c r="I15" s="34">
+        <f>'Count-&gt;Actual Activity'!F15</f>
+        <v>0.27480279717560635</v>
+      </c>
       <c r="J15" s="34"/>
       <c r="K15" s="33">
         <v>10</v>
@@ -6894,11 +6939,11 @@
       <c r="P15" s="34"/>
       <c r="Q15" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="33" t="e">
+        <v>2.7480279717560636E-2</v>
+      </c>
+      <c r="R15" s="33">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>5.496055943512127E-5</v>
       </c>
       <c r="S15" s="33">
         <f t="shared" si="2"/>
@@ -6917,7 +6962,7 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W15" s="33">
-        <f>(U15-S15*O15)/G15</f>
+        <f t="shared" si="7"/>
         <v>0.21067607630596855</v>
       </c>
       <c r="X15" s="33">
@@ -6925,15 +6970,15 @@
       </c>
       <c r="Y15" s="33">
         <f t="shared" si="5"/>
-        <v>3326.0182798264577</v>
+        <v>3234.4173474345889</v>
       </c>
       <c r="AA15" s="33">
         <f>(Q15*G15+S15*O15-U15)/U15</f>
-        <v>-0.21113942516371362</v>
+        <v>-0.1835987068978332</v>
       </c>
       <c r="AB15" s="33">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.97245928173411955</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -6961,7 +7006,10 @@
       <c r="H16" s="34">
         <v>5</v>
       </c>
-      <c r="I16" s="34"/>
+      <c r="I16" s="34">
+        <f>'Count-&gt;Actual Activity'!F16</f>
+        <v>0.28039774732102907</v>
+      </c>
       <c r="J16" s="34"/>
       <c r="K16" s="33">
         <v>10</v>
@@ -6983,11 +7031,11 @@
       <c r="P16" s="34"/>
       <c r="Q16" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="33" t="e">
+        <v>2.8039774732102906E-2</v>
+      </c>
+      <c r="R16" s="33">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>5.6079549464205813E-5</v>
       </c>
       <c r="S16" s="33">
         <f t="shared" si="2"/>
@@ -7006,7 +7054,7 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W16" s="33">
-        <f>(U16-S16*O16)/G16</f>
+        <f t="shared" si="7"/>
         <v>0.21067607630596855</v>
       </c>
       <c r="X16" s="33">
@@ -7014,7 +7062,7 @@
       </c>
       <c r="Y16" s="33">
         <f t="shared" si="5"/>
-        <v>3326.0182798264577</v>
+        <v>3232.5523640527813</v>
       </c>
       <c r="Z16" s="33"/>
       <c r="AA16" s="33" t="s">
@@ -7022,7 +7070,7 @@
       </c>
       <c r="AB16" s="33">
         <f>Y16*E16/U16</f>
-        <v>1</v>
+        <v>0.97189855619838827</v>
       </c>
     </row>
     <row r="17" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -7103,8 +7151,8 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W17" s="33">
-        <f t="shared" si="4"/>
-        <v>6.6243553877254488E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.0187371518620041</v>
       </c>
       <c r="X17" s="33">
         <v>2.3298241351735846E-2</v>
@@ -7203,8 +7251,8 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W18" s="33">
-        <f t="shared" si="4"/>
-        <v>5.5199608807595779E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.3230982289476816</v>
       </c>
       <c r="X18" s="33">
         <v>2.3298125385430756E-2</v>
@@ -7303,8 +7351,8 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W19" s="33">
-        <f t="shared" si="4"/>
-        <v>5.4895535430127172E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.86655661331916523</v>
       </c>
       <c r="X19" s="33">
         <v>2.3298122491261654E-2</v>
@@ -7644,6 +7692,12 @@
       <c r="AB23" s="38">
         <f t="shared" si="6"/>
         <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X30">
+        <f>Y11*0.03</f>
+        <v>47.381761030392077</v>
       </c>
     </row>
   </sheetData>
@@ -7655,8 +7709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7812,27 +7866,27 @@
       </c>
       <c r="B5">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
-        <v>0</v>
+        <v>0.1106105993106226</v>
       </c>
       <c r="C5">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
-        <v>0</v>
+        <v>4.3930737446564849E-3</v>
       </c>
       <c r="D5">
         <f>AVERAGE('Bottle Results'!Y11:Y13)</f>
-        <v>1665.1142147738785</v>
+        <v>1579.5677211867178</v>
       </c>
       <c r="E5">
         <f>_xlfn.STDEV.S('Bottle Results'!Y11:Y13)</f>
-        <v>2.7847474288855413E-13</v>
+        <v>0.92482158785428159</v>
       </c>
       <c r="F5">
         <f>AVERAGE('Bottle Results'!AB11:AB13)</f>
-        <v>1</v>
+        <v>0.77857254809866328</v>
       </c>
       <c r="G5">
         <f>_xlfn.STDEV.S('Bottle Results'!AB11:AB13)</f>
-        <v>0</v>
+        <v>8.7943391624000951E-3</v>
       </c>
       <c r="H5">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
@@ -7857,19 +7911,19 @@
       </c>
       <c r="D6">
         <f>AVERAGE('Bottle Results'!Y14:Y16)</f>
-        <v>3295.8495237487973</v>
+        <v>3234.1605743602818</v>
       </c>
       <c r="E6">
         <f>_xlfn.STDEV.S('Bottle Results'!Y14:Y16)</f>
-        <v>52.253818327660468</v>
+        <v>1.4964383382056994</v>
       </c>
       <c r="F6">
         <f>AVERAGE('Bottle Results'!AB14:AB16)</f>
-        <v>0.99092946774807411</v>
+        <v>0.9723820803922435</v>
       </c>
       <c r="G6">
         <f>_xlfn.STDEV.S('Bottle Results'!AB14:AB16)</f>
-        <v>1.571062271202759E-2</v>
+        <v>4.4991885561248234E-4</v>
       </c>
       <c r="H6">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
@@ -7885,36 +7939,36 @@
         <v>500</v>
       </c>
       <c r="B7">
-        <f>AVERAGE('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
-        <v>4.4084674528744358E-2</v>
+        <f>AVERAGE('Bottle Results'!W17:W19)</f>
+        <v>1.0694639980429503</v>
       </c>
       <c r="C7">
-        <f>_xlfn.STDEV.S('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
-        <v>2.9860179390728075E-2</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!W17:W19)</f>
+        <v>0.23245961239056712</v>
       </c>
       <c r="D7">
-        <f>AVERAGE('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>13998.532901237906</v>
+        <f>AVERAGE('Bottle Results'!Y17:Y19)</f>
+        <v>13107.312902868782</v>
       </c>
       <c r="E7">
-        <f>_xlfn.STDEV.S('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>1891.3936416951028</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!Y17:Y19)</f>
+        <v>774.8653746352262</v>
       </c>
       <c r="F7">
-        <f>AVERAGE('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>0.83963357359586033</v>
+        <f>AVERAGE('Bottle Results'!AB17:AB19)</f>
+        <v>0.78617809812781381</v>
       </c>
       <c r="G7">
-        <f>_xlfn.STDEV.S('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>0.11344600278165595</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!AB17:AB19)</f>
+        <v>4.6476512085286893E-2</v>
       </c>
       <c r="H7">
-        <f>AVERAGE('Bottle Results'!D17:D19,'Bottle Results'!D21)</f>
-        <v>8.9350000000000005</v>
+        <f>AVERAGE('Bottle Results'!D17:D19)</f>
+        <v>8.913333333333334</v>
       </c>
       <c r="I7">
-        <f>_xlfn.STDEV.S('Bottle Results'!D17:D19,'Bottle Results'!D21)</f>
-        <v>4.7258156262525892E-2</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!D17:D19)</f>
+        <v>2.3094010767584539E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Added pyrite, 50 Bq FHY pH9"
This reverts commit c3d8368848a1aeb9bc0922aa94cccb2d534bf452.
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -2646,7 +2646,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,23 +3432,16 @@
       <c r="B33" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="21">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="D33" s="21">
-        <f>C33*3.8/100</f>
-        <v>2.2040000000000002E-3</v>
-      </c>
       <c r="E33" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F33" s="1">
         <f>(C33-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>39.146000743058828</v>
+        <v>-4.9863554343643806</v>
       </c>
       <c r="G33" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F33-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>567.79850308782375</v>
+        <v>74.035276446395159</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3458,23 +3451,16 @@
       <c r="B34" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="21">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="D34" s="21">
-        <f>3.2/100*C34</f>
-        <v>1.8240000000000001E-3</v>
-      </c>
       <c r="E34" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F34" s="1">
         <f>(C34-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>38.385098050344638</v>
+        <v>-4.9863554343643806</v>
       </c>
       <c r="G34" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F34-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>556.73647081686329</v>
+        <v>74.035276446395159</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3484,23 +3470,16 @@
       <c r="B35" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="21">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="D35" s="21">
-        <f>3.6/100*C35</f>
-        <v>2.0880000000000004E-3</v>
-      </c>
       <c r="E35" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F35" s="1">
         <f>(C35-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>39.146000743058828</v>
+        <v>-4.9863554343643806</v>
       </c>
       <c r="G35" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F35-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>567.79850308782375</v>
+        <v>74.035276446395159</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -5587,10 +5566,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6515,283 +6494,262 @@
         <v>0.64413205376649052</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11">
         <v>2E-3</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11">
         <v>8.94</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="1">
         <v>0.03</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="21">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="1">
         <v>100</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="1">
         <v>5</v>
       </c>
-      <c r="I11" s="34">
-        <f>'Count-&gt;Actual Activity'!F11</f>
-        <v>0.25716654128242811</v>
-      </c>
-      <c r="J11" s="34"/>
-      <c r="K11" s="33">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11">
         <v>10</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11">
         <v>0.02</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="1">
         <f>'Count-&gt;Actual Activity'!F33</f>
-        <v>39.146000743058828</v>
-      </c>
-      <c r="N11" s="34">
+        <v>-4.9863554343643806</v>
+      </c>
+      <c r="N11" s="1">
         <f>'Count-&gt;Actual Activity'!G33</f>
-        <v>567.79850308782375</v>
-      </c>
-      <c r="O11" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="P11" s="33">
-        <v>9.0000000000000006E-5</v>
-      </c>
-      <c r="Q11" s="33">
+        <v>74.035276446395159</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11">
         <f t="shared" si="0"/>
-        <v>2.5716654128242811E-2</v>
-      </c>
-      <c r="R11" s="33">
+        <v>0</v>
+      </c>
+      <c r="R11" t="e">
         <f t="shared" si="1"/>
-        <v>5.1433308256485625E-5</v>
-      </c>
-      <c r="S11" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S11" t="e">
         <f t="shared" si="2"/>
-        <v>1304.8666914352943</v>
-      </c>
-      <c r="T11" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T11" t="e">
         <f t="shared" si="3"/>
-        <v>18926.75171217525</v>
-      </c>
-      <c r="U11" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U11">
         <f>Parameters!$B$6*'Bottle Results'!B11</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V11" s="33">
+      <c r="V11">
         <f>SQRT((C11/B11)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W11" s="33">
-        <f t="shared" ref="W11:W19" si="7">(U11-S11*O11)/G11</f>
-        <v>0.1080742570015753</v>
-      </c>
-      <c r="X11" s="33">
+      <c r="W11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X11">
         <v>2.3297919246001962E-2</v>
       </c>
-      <c r="Y11" s="33">
+      <c r="Y11">
         <f t="shared" si="5"/>
-        <v>1579.3920343464026</v>
-      </c>
-      <c r="AA11" s="33" t="s">
+        <v>1665.1142147738788</v>
+      </c>
+      <c r="AA11" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AB11" s="33">
-        <f>S11*E11/U11</f>
-        <v>0.78364996218141969</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="AB11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12">
         <v>2E-3</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12">
         <v>8.89</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="1">
         <v>0.03</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="21">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="1">
         <v>100</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="1">
         <v>5</v>
       </c>
-      <c r="I12" s="34">
-        <f>'Count-&gt;Actual Activity'!F12</f>
-        <v>0.25363929010379288</v>
-      </c>
-      <c r="J12" s="34"/>
-      <c r="K12" s="33">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12">
         <v>10</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12">
         <v>0.02</v>
       </c>
-      <c r="M12" s="34">
+      <c r="M12" s="1">
         <f>'Count-&gt;Actual Activity'!F34</f>
-        <v>38.385098050344638</v>
-      </c>
-      <c r="N12" s="34">
+        <v>-4.9863554343643806</v>
+      </c>
+      <c r="N12" s="1">
         <f>'Count-&gt;Actual Activity'!G34</f>
-        <v>556.73647081686329</v>
-      </c>
-      <c r="O12" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="P12" s="33">
-        <v>9.0000000000000006E-5</v>
-      </c>
-      <c r="Q12" s="33">
+        <v>74.035276446395159</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12">
         <f t="shared" si="0"/>
-        <v>2.5363929010379288E-2</v>
-      </c>
-      <c r="R12" s="33">
+        <v>0</v>
+      </c>
+      <c r="R12" t="e">
         <f t="shared" si="1"/>
-        <v>5.072785802075858E-5</v>
-      </c>
-      <c r="S12" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S12" t="e">
         <f t="shared" si="2"/>
-        <v>1279.5032683448212</v>
-      </c>
-      <c r="T12" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T12" t="e">
         <f t="shared" si="3"/>
-        <v>18558.014686229326</v>
-      </c>
-      <c r="U12" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U12">
         <f>Parameters!$B$6*'Bottle Results'!B12</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V12" s="33">
+      <c r="V12">
         <f>SQRT((C12/B12)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W12" s="33">
-        <f t="shared" si="7"/>
-        <v>0.1156832839287172</v>
-      </c>
-      <c r="X12" s="33">
+      <c r="W12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X12">
         <v>2.3297917690924E-2</v>
       </c>
-      <c r="Y12" s="33">
+      <c r="Y12">
         <f t="shared" si="5"/>
-        <v>1580.567784739281</v>
-      </c>
-      <c r="AA12" s="33" t="s">
+        <v>1665.1142147738788</v>
+      </c>
+      <c r="AA12" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AB12" s="33">
-        <f>S12*E12/U12</f>
-        <v>0.76841771993315</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="AB12">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13">
         <v>2E-3</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13">
         <v>8.92</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="1">
         <v>0.03</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="21">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="1">
         <v>100</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="1">
         <v>5</v>
       </c>
-      <c r="I13" s="34">
-        <f>'Count-&gt;Actual Activity'!F13</f>
-        <v>0.25911261089822724</v>
-      </c>
-      <c r="J13" s="34"/>
-      <c r="K13" s="33">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13">
         <v>10</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13">
         <v>0.02</v>
       </c>
-      <c r="M13" s="34">
+      <c r="M13" s="1">
         <f>'Count-&gt;Actual Activity'!F35</f>
-        <v>39.146000743058828</v>
-      </c>
-      <c r="N13" s="34">
+        <v>-4.9863554343643806</v>
+      </c>
+      <c r="N13" s="1">
         <f>'Count-&gt;Actual Activity'!G35</f>
-        <v>567.79850308782375</v>
-      </c>
-      <c r="O13" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="P13" s="33">
-        <v>9.0000000000000006E-5</v>
-      </c>
-      <c r="Q13" s="33">
+        <v>74.035276446395159</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13">
         <f t="shared" si="0"/>
-        <v>2.5911261089822724E-2</v>
-      </c>
-      <c r="R13" s="33">
+        <v>0</v>
+      </c>
+      <c r="R13" t="e">
         <f t="shared" si="1"/>
-        <v>5.182252217964545E-5</v>
-      </c>
-      <c r="S13" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S13" t="e">
         <f t="shared" si="2"/>
-        <v>1304.8666914352943</v>
-      </c>
-      <c r="T13" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T13" t="e">
         <f t="shared" si="3"/>
-        <v>18926.75171217525</v>
-      </c>
-      <c r="U13" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U13">
         <f>Parameters!$B$6*'Bottle Results'!B13</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V13" s="33">
+      <c r="V13">
         <f>SQRT((C13/B13)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W13" s="33">
-        <f t="shared" si="7"/>
-        <v>0.1080742570015753</v>
-      </c>
-      <c r="X13" s="33">
+      <c r="W13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X13">
         <v>2.3297920113197729E-2</v>
       </c>
-      <c r="Y13" s="33">
+      <c r="Y13">
         <f t="shared" si="5"/>
-        <v>1578.7433444744695</v>
-      </c>
-      <c r="AA13" s="33" t="s">
+        <v>1665.1142147738788</v>
+      </c>
+      <c r="AA13" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="AB13" s="33">
-        <f>S13*E13/U13</f>
-        <v>0.78364996218141969</v>
+      <c r="AB13">
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -6870,7 +6828,7 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W14" s="33">
-        <f t="shared" si="7"/>
+        <f>(U14-S14*O14)/G14</f>
         <v>0.21067607630596855</v>
       </c>
       <c r="X14" s="33">
@@ -6914,10 +6872,7 @@
       <c r="H15" s="34">
         <v>5</v>
       </c>
-      <c r="I15" s="34">
-        <f>'Count-&gt;Actual Activity'!F15</f>
-        <v>0.27480279717560635</v>
-      </c>
+      <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="33">
         <v>10</v>
@@ -6939,11 +6894,11 @@
       <c r="P15" s="34"/>
       <c r="Q15" s="33">
         <f t="shared" si="0"/>
-        <v>2.7480279717560636E-2</v>
-      </c>
-      <c r="R15" s="33">
+        <v>0</v>
+      </c>
+      <c r="R15" s="33" t="e">
         <f t="shared" si="1"/>
-        <v>5.496055943512127E-5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S15" s="33">
         <f t="shared" si="2"/>
@@ -6962,7 +6917,7 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W15" s="33">
-        <f t="shared" si="7"/>
+        <f>(U15-S15*O15)/G15</f>
         <v>0.21067607630596855</v>
       </c>
       <c r="X15" s="33">
@@ -6970,15 +6925,15 @@
       </c>
       <c r="Y15" s="33">
         <f t="shared" si="5"/>
-        <v>3234.4173474345889</v>
+        <v>3326.0182798264577</v>
       </c>
       <c r="AA15" s="33">
         <f>(Q15*G15+S15*O15-U15)/U15</f>
-        <v>-0.1835987068978332</v>
+        <v>-0.21113942516371362</v>
       </c>
       <c r="AB15" s="33">
         <f t="shared" si="6"/>
-        <v>0.97245928173411955</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -7006,10 +6961,7 @@
       <c r="H16" s="34">
         <v>5</v>
       </c>
-      <c r="I16" s="34">
-        <f>'Count-&gt;Actual Activity'!F16</f>
-        <v>0.28039774732102907</v>
-      </c>
+      <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="33">
         <v>10</v>
@@ -7031,11 +6983,11 @@
       <c r="P16" s="34"/>
       <c r="Q16" s="33">
         <f t="shared" si="0"/>
-        <v>2.8039774732102906E-2</v>
-      </c>
-      <c r="R16" s="33">
+        <v>0</v>
+      </c>
+      <c r="R16" s="33" t="e">
         <f t="shared" si="1"/>
-        <v>5.6079549464205813E-5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S16" s="33">
         <f t="shared" si="2"/>
@@ -7054,7 +7006,7 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W16" s="33">
-        <f t="shared" si="7"/>
+        <f>(U16-S16*O16)/G16</f>
         <v>0.21067607630596855</v>
       </c>
       <c r="X16" s="33">
@@ -7062,7 +7014,7 @@
       </c>
       <c r="Y16" s="33">
         <f t="shared" si="5"/>
-        <v>3232.5523640527813</v>
+        <v>3326.0182798264577</v>
       </c>
       <c r="Z16" s="33"/>
       <c r="AA16" s="33" t="s">
@@ -7070,7 +7022,7 @@
       </c>
       <c r="AB16" s="33">
         <f>Y16*E16/U16</f>
-        <v>0.97189855619838827</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -7151,8 +7103,8 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W17" s="33">
-        <f t="shared" si="7"/>
-        <v>1.0187371518620041</v>
+        <f t="shared" si="4"/>
+        <v>6.6243553877254488E-2</v>
       </c>
       <c r="X17" s="33">
         <v>2.3298241351735846E-2</v>
@@ -7251,8 +7203,8 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W18" s="33">
-        <f t="shared" si="7"/>
-        <v>1.3230982289476816</v>
+        <f t="shared" si="4"/>
+        <v>5.5199608807595779E-2</v>
       </c>
       <c r="X18" s="33">
         <v>2.3298125385430756E-2</v>
@@ -7351,8 +7303,8 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W19" s="33">
-        <f t="shared" si="7"/>
-        <v>0.86655661331916523</v>
+        <f t="shared" si="4"/>
+        <v>5.4895535430127172E-2</v>
       </c>
       <c r="X19" s="33">
         <v>2.3298122491261654E-2</v>
@@ -7692,12 +7644,6 @@
       <c r="AB23" s="38">
         <f t="shared" si="6"/>
         <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="X30">
-        <f>Y11*0.03</f>
-        <v>47.381761030392077</v>
       </c>
     </row>
   </sheetData>
@@ -7709,8 +7655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7866,27 +7812,27 @@
       </c>
       <c r="B5">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
-        <v>0.1106105993106226</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
-        <v>4.3930737446564849E-3</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f>AVERAGE('Bottle Results'!Y11:Y13)</f>
-        <v>1579.5677211867178</v>
+        <v>1665.1142147738785</v>
       </c>
       <c r="E5">
         <f>_xlfn.STDEV.S('Bottle Results'!Y11:Y13)</f>
-        <v>0.92482158785428159</v>
+        <v>2.7847474288855413E-13</v>
       </c>
       <c r="F5">
         <f>AVERAGE('Bottle Results'!AB11:AB13)</f>
-        <v>0.77857254809866328</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f>_xlfn.STDEV.S('Bottle Results'!AB11:AB13)</f>
-        <v>8.7943391624000951E-3</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
@@ -7911,19 +7857,19 @@
       </c>
       <c r="D6">
         <f>AVERAGE('Bottle Results'!Y14:Y16)</f>
-        <v>3234.1605743602818</v>
+        <v>3295.8495237487973</v>
       </c>
       <c r="E6">
         <f>_xlfn.STDEV.S('Bottle Results'!Y14:Y16)</f>
-        <v>1.4964383382056994</v>
+        <v>52.253818327660468</v>
       </c>
       <c r="F6">
         <f>AVERAGE('Bottle Results'!AB14:AB16)</f>
-        <v>0.9723820803922435</v>
+        <v>0.99092946774807411</v>
       </c>
       <c r="G6">
         <f>_xlfn.STDEV.S('Bottle Results'!AB14:AB16)</f>
-        <v>4.4991885561248234E-4</v>
+        <v>1.571062271202759E-2</v>
       </c>
       <c r="H6">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
@@ -7939,36 +7885,36 @@
         <v>500</v>
       </c>
       <c r="B7">
-        <f>AVERAGE('Bottle Results'!W17:W19)</f>
-        <v>1.0694639980429503</v>
+        <f>AVERAGE('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
+        <v>4.4084674528744358E-2</v>
       </c>
       <c r="C7">
-        <f>_xlfn.STDEV.S('Bottle Results'!W17:W19)</f>
-        <v>0.23245961239056712</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
+        <v>2.9860179390728075E-2</v>
       </c>
       <c r="D7">
-        <f>AVERAGE('Bottle Results'!Y17:Y19)</f>
-        <v>13107.312902868782</v>
+        <f>AVERAGE('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
+        <v>13998.532901237906</v>
       </c>
       <c r="E7">
-        <f>_xlfn.STDEV.S('Bottle Results'!Y17:Y19)</f>
-        <v>774.8653746352262</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
+        <v>1891.3936416951028</v>
       </c>
       <c r="F7">
-        <f>AVERAGE('Bottle Results'!AB17:AB19)</f>
-        <v>0.78617809812781381</v>
+        <f>AVERAGE('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
+        <v>0.83963357359586033</v>
       </c>
       <c r="G7">
-        <f>_xlfn.STDEV.S('Bottle Results'!AB17:AB19)</f>
-        <v>4.6476512085286893E-2</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
+        <v>0.11344600278165595</v>
       </c>
       <c r="H7">
-        <f>AVERAGE('Bottle Results'!D17:D19)</f>
-        <v>8.913333333333334</v>
+        <f>AVERAGE('Bottle Results'!D17:D19,'Bottle Results'!D21)</f>
+        <v>8.9350000000000005</v>
       </c>
       <c r="I7">
-        <f>_xlfn.STDEV.S('Bottle Results'!D17:D19)</f>
-        <v>2.3094010767584539E-2</v>
+        <f>_xlfn.STDEV.S('Bottle Results'!D17:D19,'Bottle Results'!D21)</f>
+        <v>4.7258156262525892E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edit manuscript, Need to recalculate ALL values
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -2645,8 +2645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A6" zoomScale="79" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,16 +3432,23 @@
       <c r="B33" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="C33" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D33" s="21">
+        <f>3.8/100*C33</f>
+        <v>2.2040000000000002E-3</v>
+      </c>
       <c r="E33" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F33" s="1">
         <f>(C33-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>-4.9863554343643806</v>
+        <v>39.146000743058828</v>
       </c>
       <c r="G33" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F33-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>74.035276446395159</v>
+        <v>567.79850308782375</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3451,16 +3458,23 @@
       <c r="B34" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="C34" s="21">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D34" s="21">
+        <f>3.2/100*C34</f>
+        <v>1.8240000000000001E-3</v>
+      </c>
       <c r="E34" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F34" s="1">
         <f>(C34-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>-4.9863554343643806</v>
+        <v>38.385098050344638</v>
       </c>
       <c r="G34" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F34-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>74.035276446395159</v>
+        <v>556.73647081686329</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3470,16 +3484,23 @@
       <c r="B35" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="C35" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D35" s="21">
+        <f>3.6/100*C35</f>
+        <v>2.0880000000000004E-3</v>
+      </c>
       <c r="E35" s="31" t="s">
         <v>151</v>
       </c>
       <c r="F35" s="1">
         <f>(C35-'Calibration data'!$L$64)/'Calibration data'!$L$65</f>
-        <v>-4.9863554343643806</v>
+        <v>39.146000743058828</v>
       </c>
       <c r="G35" s="22">
         <f>'Calibration data'!$L$54/'Calibration data'!$L$65*SQRT(1/'Calibration data'!$L$55+1+('Count-&gt;Actual Activity'!F35-AVERAGE('Calibration data'!$F$3:$F$8))^2/('Calibration data'!$L$65^2*'Calibration data'!$J$9))</f>
-        <v>74.035276446395159</v>
+        <v>567.79850308782375</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -5568,8 +5589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5848,7 +5869,7 @@
         <v>2.3297922254460427E-2</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y16" si="5">(U3-Q3*G3)/E3</f>
+        <f t="shared" ref="Y3:Y7" si="5">(U3-Q3*G3)/E3</f>
         <v>0</v>
       </c>
       <c r="AA3" t="s">
@@ -6288,7 +6309,7 @@
         <v>2.3297913974600508E-2</v>
       </c>
       <c r="Y8" s="33">
-        <f>S8</f>
+        <f t="shared" ref="Y8:Y19" si="7">S8</f>
         <v>239.60292163542371</v>
       </c>
       <c r="AA8" s="33">
@@ -6385,7 +6406,7 @@
         <v>2.3297916895026565E-2</v>
       </c>
       <c r="Y9" s="33">
-        <f>S9</f>
+        <f t="shared" si="7"/>
         <v>239.60292163542371</v>
       </c>
       <c r="AA9" s="33">
@@ -6482,7 +6503,7 @@
         <v>2.3297919570431896E-2</v>
       </c>
       <c r="Y10" s="33">
-        <f>S10</f>
+        <f t="shared" si="7"/>
         <v>214.23949854495061</v>
       </c>
       <c r="AA10" s="33">
@@ -6494,262 +6515,268 @@
         <v>0.64413205376649052</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="33">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="33">
         <v>2E-3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="33">
         <v>8.94</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="34">
         <v>0.03</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="35">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="34">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="34">
         <v>5</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11">
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="33">
         <v>10</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="33">
         <v>0.02</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="34">
         <f>'Count-&gt;Actual Activity'!F33</f>
-        <v>-4.9863554343643806</v>
-      </c>
-      <c r="N11" s="1">
+        <v>39.146000743058828</v>
+      </c>
+      <c r="N11" s="34">
         <f>'Count-&gt;Actual Activity'!G33</f>
-        <v>74.035276446395159</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11">
+        <v>567.79850308782375</v>
+      </c>
+      <c r="O11" s="34">
+        <v>0.03</v>
+      </c>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R11" t="e">
+      <c r="R11" s="33" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S11" t="e">
+      <c r="S11" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T11" t="e">
+        <v>1304.8666914352943</v>
+      </c>
+      <c r="T11" s="33">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U11">
+        <v>18926.616769594126</v>
+      </c>
+      <c r="U11" s="33">
         <f>Parameters!$B$6*'Bottle Results'!B11</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="33">
         <f>SQRT((C11/B11)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X11">
+      <c r="W11" s="33">
+        <f t="shared" ref="W11:W19" si="8">(U11-S11*O11)/G11</f>
+        <v>0.1080742570015753</v>
+      </c>
+      <c r="X11" s="33">
         <v>2.3297919246001962E-2</v>
       </c>
-      <c r="Y11">
-        <f t="shared" si="5"/>
-        <v>1665.1142147738788</v>
-      </c>
-      <c r="AA11" s="38" t="s">
+      <c r="Y11" s="33">
+        <f t="shared" si="7"/>
+        <v>1304.8666914352943</v>
+      </c>
+      <c r="AA11" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="33">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+        <v>0.78364996218141969</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="33">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="33">
         <v>2E-3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="33">
         <v>8.89</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="34">
         <v>0.03</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="35">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="34">
         <v>100</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="34">
         <v>5</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12">
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="33">
         <v>10</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="33">
         <v>0.02</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="34">
         <f>'Count-&gt;Actual Activity'!F34</f>
-        <v>-4.9863554343643806</v>
-      </c>
-      <c r="N12" s="1">
+        <v>38.385098050344638</v>
+      </c>
+      <c r="N12" s="34">
         <f>'Count-&gt;Actual Activity'!G34</f>
-        <v>74.035276446395159</v>
-      </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12">
+        <v>556.73647081686329</v>
+      </c>
+      <c r="O12" s="34">
+        <v>0.03</v>
+      </c>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R12" t="e">
+      <c r="R12" s="33" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S12" t="e">
+      <c r="S12" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T12" t="e">
+        <v>1279.5032683448212</v>
+      </c>
+      <c r="T12" s="33">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U12">
+        <v>18557.882360562107</v>
+      </c>
+      <c r="U12" s="33">
         <f>Parameters!$B$6*'Bottle Results'!B12</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="33">
         <f>SQRT((C12/B12)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X12">
+      <c r="W12" s="33">
+        <f t="shared" si="8"/>
+        <v>0.1156832839287172</v>
+      </c>
+      <c r="X12" s="33">
         <v>2.3297917690924E-2</v>
       </c>
-      <c r="Y12">
-        <f t="shared" si="5"/>
-        <v>1665.1142147738788</v>
-      </c>
-      <c r="AA12" s="38" t="s">
+      <c r="Y12" s="33">
+        <f t="shared" si="7"/>
+        <v>1279.5032683448212</v>
+      </c>
+      <c r="AA12" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="33">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+        <v>0.76841771993315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="33">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="33">
         <v>2E-3</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="33">
         <v>8.92</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="34">
         <v>0.03</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="35">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="34">
         <v>100</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="34">
         <v>5</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13">
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="33">
         <v>10</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="33">
         <v>0.02</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="34">
         <f>'Count-&gt;Actual Activity'!F35</f>
-        <v>-4.9863554343643806</v>
-      </c>
-      <c r="N13" s="1">
+        <v>39.146000743058828</v>
+      </c>
+      <c r="N13" s="34">
         <f>'Count-&gt;Actual Activity'!G35</f>
-        <v>74.035276446395159</v>
-      </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13">
+        <v>567.79850308782375</v>
+      </c>
+      <c r="O13" s="34">
+        <v>0.03</v>
+      </c>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R13" t="e">
+      <c r="R13" s="33" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S13" t="e">
+      <c r="S13" s="33">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T13" t="e">
+        <v>1304.8666914352943</v>
+      </c>
+      <c r="T13" s="33">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13">
+        <v>18926.616769594126</v>
+      </c>
+      <c r="U13" s="33">
         <f>Parameters!$B$6*'Bottle Results'!B13</f>
         <v>49.953426443216358</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="33">
         <f>SQRT((C13/B13)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.8486259533798084E-2</v>
       </c>
-      <c r="W13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X13">
+      <c r="W13" s="33">
+        <f t="shared" si="8"/>
+        <v>0.1080742570015753</v>
+      </c>
+      <c r="X13" s="33">
         <v>2.3297920113197729E-2</v>
       </c>
-      <c r="Y13">
-        <f t="shared" si="5"/>
-        <v>1665.1142147738788</v>
-      </c>
-      <c r="AA13" s="38" t="s">
+      <c r="Y13" s="33">
+        <f t="shared" si="7"/>
+        <v>1304.8666914352943</v>
+      </c>
+      <c r="AA13" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="33">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.78364996218141969</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -6828,15 +6855,15 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W14" s="33">
-        <f>(U14-S14*O14)/G14</f>
+        <f t="shared" si="8"/>
         <v>0.21067607630596855</v>
       </c>
       <c r="X14" s="33">
         <v>2.3297925795726985E-2</v>
       </c>
       <c r="Y14" s="33">
-        <f t="shared" si="5"/>
-        <v>3235.512011593476</v>
+        <f t="shared" si="7"/>
+        <v>2623.7646921398959</v>
       </c>
       <c r="AA14" s="33">
         <f>(Q14*G14+S14*O14-U14)/U14</f>
@@ -6844,7 +6871,7 @@
       </c>
       <c r="AB14" s="33">
         <f t="shared" si="6"/>
-        <v>0.97278840324422267</v>
+        <v>0.78886057483628635</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -6917,15 +6944,15 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W15" s="33">
-        <f>(U15-S15*O15)/G15</f>
+        <f t="shared" si="8"/>
         <v>0.21067607630596855</v>
       </c>
       <c r="X15" s="33">
         <v>2.329792734453592E-2</v>
       </c>
       <c r="Y15" s="33">
-        <f t="shared" si="5"/>
-        <v>3326.0182798264577</v>
+        <f t="shared" si="7"/>
+        <v>2623.7646921398959</v>
       </c>
       <c r="AA15" s="33">
         <f>(Q15*G15+S15*O15-U15)/U15</f>
@@ -6933,7 +6960,7 @@
       </c>
       <c r="AB15" s="33">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.78886057483628635</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -7006,15 +7033,15 @@
         <v>3.165627094523759E-2</v>
       </c>
       <c r="W16" s="33">
-        <f>(U16-S16*O16)/G16</f>
+        <f t="shared" si="8"/>
         <v>0.21067607630596855</v>
       </c>
       <c r="X16" s="33">
         <v>2.3297930026256426E-2</v>
       </c>
       <c r="Y16" s="33">
-        <f t="shared" si="5"/>
-        <v>3326.0182798264577</v>
+        <f t="shared" si="7"/>
+        <v>2623.7646921398959</v>
       </c>
       <c r="Z16" s="33"/>
       <c r="AA16" s="33" t="s">
@@ -7022,7 +7049,7 @@
       </c>
       <c r="AB16" s="33">
         <f>Y16*E16/U16</f>
-        <v>1</v>
+        <v>0.78886057483628635</v>
       </c>
     </row>
     <row r="17" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -7103,14 +7130,14 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W17" s="33">
-        <f t="shared" si="4"/>
-        <v>6.6243553877254488E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.0187371518620041</v>
       </c>
       <c r="X17" s="33">
         <v>2.3298241351735846E-2</v>
       </c>
       <c r="Y17" s="33">
-        <f>S17</f>
+        <f t="shared" si="7"/>
         <v>13276.402390138603</v>
       </c>
       <c r="Z17" s="33">
@@ -7203,14 +7230,14 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W18" s="33">
-        <f t="shared" si="4"/>
-        <v>5.5199608807595779E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.3230982289476816</v>
       </c>
       <c r="X18" s="33">
         <v>2.3298125385430756E-2</v>
       </c>
       <c r="Y18" s="33">
-        <f>S18</f>
+        <f t="shared" si="7"/>
         <v>12261.865466519677</v>
       </c>
       <c r="Z18" s="33">
@@ -7303,14 +7330,14 @@
         <v>2.9125000570302848E-2</v>
       </c>
       <c r="W19" s="33">
-        <f t="shared" si="4"/>
-        <v>5.4895535430127172E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.86655661331916523</v>
       </c>
       <c r="X19" s="33">
         <v>2.3298122491261654E-2</v>
       </c>
       <c r="Y19" s="33">
-        <f>S19</f>
+        <f t="shared" si="7"/>
         <v>13783.670851948065</v>
       </c>
       <c r="AA19" s="33">
@@ -7434,7 +7461,10 @@
       <c r="H21" s="39">
         <v>5</v>
       </c>
-      <c r="I21" s="39"/>
+      <c r="I21" s="39">
+        <f>'Count-&gt;Actual Activity'!F20</f>
+        <v>1.0942501421156658</v>
+      </c>
       <c r="J21" s="39"/>
       <c r="K21" s="38">
         <v>10</v>
@@ -7442,14 +7472,8 @@
       <c r="L21" s="38">
         <v>0.02</v>
       </c>
-      <c r="M21" s="39">
-        <f>'Count-&gt;Actual Activity'!F43</f>
-        <v>-0.49702954735064037</v>
-      </c>
-      <c r="N21" s="39">
-        <f>'Count-&gt;Actual Activity'!G43</f>
-        <v>10.045075299214339</v>
-      </c>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
       <c r="O21" s="38">
         <v>0.03</v>
       </c>
@@ -7458,11 +7482,11 @@
       </c>
       <c r="Q21" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="38" t="e">
+        <v>0.10942501421156658</v>
+      </c>
+      <c r="R21" s="38">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.1885002842313318E-4</v>
       </c>
       <c r="U21" s="38">
         <f>Parameters!$B$6*'Bottle Results'!B21</f>
@@ -7474,18 +7498,18 @@
       </c>
       <c r="W21" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.10942501421156658</v>
       </c>
       <c r="X21" s="38">
         <v>2.3298893977915368E-2</v>
       </c>
       <c r="Y21" s="38">
         <f>(U21-Q21*G21)/E21</f>
-        <v>16672.192896345281</v>
+        <v>16307.442848973395</v>
       </c>
       <c r="AB21" s="38">
         <f t="shared" si="6"/>
-        <v>0.99999999999999989</v>
+        <v>0.97812225124555485</v>
       </c>
     </row>
     <row r="22" spans="1:28" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -7655,8 +7679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7812,27 +7836,27 @@
       </c>
       <c r="B5">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
-        <v>0</v>
+        <v>0.1106105993106226</v>
       </c>
       <c r="C5">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
-        <v>0</v>
+        <v>4.3930737446564849E-3</v>
       </c>
       <c r="D5">
         <f>AVERAGE('Bottle Results'!Y11:Y13)</f>
-        <v>1665.1142147738785</v>
+        <v>1296.4122170718033</v>
       </c>
       <c r="E5">
         <f>_xlfn.STDEV.S('Bottle Results'!Y11:Y13)</f>
-        <v>2.7847474288855413E-13</v>
+        <v>14.643579148855034</v>
       </c>
       <c r="F5">
         <f>AVERAGE('Bottle Results'!AB11:AB13)</f>
-        <v>1</v>
+        <v>0.77857254809866328</v>
       </c>
       <c r="G5">
         <f>_xlfn.STDEV.S('Bottle Results'!AB11:AB13)</f>
-        <v>0</v>
+        <v>8.7943391624000951E-3</v>
       </c>
       <c r="H5">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
@@ -7857,19 +7881,19 @@
       </c>
       <c r="D6">
         <f>AVERAGE('Bottle Results'!Y14:Y16)</f>
-        <v>3295.8495237487973</v>
+        <v>2623.7646921398959</v>
       </c>
       <c r="E6">
         <f>_xlfn.STDEV.S('Bottle Results'!Y14:Y16)</f>
-        <v>52.253818327660468</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>AVERAGE('Bottle Results'!AB14:AB16)</f>
-        <v>0.99092946774807411</v>
+        <v>0.78886057483628635</v>
       </c>
       <c r="G6">
         <f>_xlfn.STDEV.S('Bottle Results'!AB14:AB16)</f>
-        <v>1.571062271202759E-2</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
@@ -7886,27 +7910,27 @@
       </c>
       <c r="B7">
         <f>AVERAGE('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
-        <v>4.4084674528744358E-2</v>
+        <v>0.82945425208510437</v>
       </c>
       <c r="C7">
         <f>_xlfn.STDEV.S('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
-        <v>2.9860179390728075E-2</v>
+        <v>0.51618184155151592</v>
       </c>
       <c r="D7">
         <f>AVERAGE('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>13998.532901237906</v>
+        <v>13907.345389394934</v>
       </c>
       <c r="E7">
         <f>_xlfn.STDEV.S('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>1891.3936416951028</v>
+        <v>1720.6061385050698</v>
       </c>
       <c r="F7">
         <f>AVERAGE('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>0.83963357359586033</v>
+        <v>0.83416413640724907</v>
       </c>
       <c r="G7">
         <f>_xlfn.STDEV.S('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>0.11344600278165595</v>
+        <v>0.10320214918352018</v>
       </c>
       <c r="H7">
         <f>AVERAGE('Bottle Results'!D17:D19,'Bottle Results'!D21)</f>

</xml_diff>

<commit_message>
Updated RaFHYpH9 Solid Counts
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="147">
   <si>
     <t>Parameters</t>
   </si>
@@ -2581,7 +2581,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,14 +3178,8 @@
       <c r="E24" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F24" s="1" t="e">
-        <f>(C24-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G24" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!L65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F24-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
@@ -3197,14 +3191,8 @@
       <c r="E25" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F25" s="1" t="e">
-        <f>(C25-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F25-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
@@ -3216,14 +3204,8 @@
       <c r="E26" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F26" s="1" t="e">
-        <f>(C26-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G26" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F26-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
@@ -3235,13 +3217,11 @@
       <c r="E27" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F27" s="1" t="e">
-        <f>(C27-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F27-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F27" s="1">
+        <v>2.7749999999999999</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0.25219999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3254,13 +3234,11 @@
       <c r="E28" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F28" s="1" t="e">
-        <f>(C28-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F28-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F28" s="1">
+        <v>3.2250000000000001</v>
+      </c>
+      <c r="G28" s="16">
+        <v>0.2591</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3273,14 +3251,8 @@
       <c r="E29" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F29" s="1" t="e">
-        <f>(C29-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F29-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
@@ -3289,23 +3261,16 @@
       <c r="B30" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C30" s="15">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D30" s="15">
-        <f>0.052*C30</f>
-        <v>8.3199999999999995E-4</v>
-      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
       <c r="E30" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F30" s="1" t="e">
-        <f>(C30-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F30-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F30" s="1">
+        <v>6.1120000000000001</v>
+      </c>
+      <c r="G30" s="16">
+        <v>0.32490000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3315,23 +3280,16 @@
       <c r="B31" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="15">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D31" s="15">
-        <f>0.045*C31</f>
-        <v>7.1999999999999994E-4</v>
-      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
       <c r="E31" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F31" s="1" t="e">
-        <f>(C31-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G31" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F31-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F31" s="1">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="G31" s="16">
+        <v>0.3201</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3341,23 +3299,16 @@
       <c r="B32" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D32" s="15">
-        <f>0.064*C32</f>
-        <v>9.6000000000000002E-4</v>
-      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
       <c r="E32" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F32" s="1" t="e">
-        <f>(C32-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G32" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F32-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F32" s="1">
+        <v>5.6020000000000003</v>
+      </c>
+      <c r="G32" s="16">
+        <v>0.37659999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3367,23 +3318,16 @@
       <c r="B33" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="15">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="D33" s="15">
-        <f>3.8/100*C33</f>
-        <v>2.2040000000000002E-3</v>
-      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F33" s="1" t="e">
-        <f>(C33-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G33" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F33-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F33" s="1">
+        <v>21.28</v>
+      </c>
+      <c r="G33" s="16">
+        <v>1.0509999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3393,23 +3337,16 @@
       <c r="B34" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="15">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="D34" s="15">
-        <f>3.2/100*C34</f>
-        <v>1.8240000000000001E-3</v>
-      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
       <c r="E34" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F34" s="1" t="e">
-        <f>(C34-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G34" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F34-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F34" s="1">
+        <v>20.83</v>
+      </c>
+      <c r="G34" s="16">
+        <v>0.94069999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3419,23 +3356,16 @@
       <c r="B35" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="15">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="D35" s="15">
-        <f>3.6/100*C35</f>
-        <v>2.0880000000000004E-3</v>
-      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
       <c r="E35" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F35" s="1" t="e">
-        <f>(C35-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G35" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F35-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F35" s="1">
+        <v>21.45</v>
+      </c>
+      <c r="G35" s="16">
+        <v>1.032</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3445,23 +3375,14 @@
       <c r="B36" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C36">
-        <v>0.11</v>
-      </c>
-      <c r="D36">
-        <f>2.7/100*C36</f>
-        <v>2.9700000000000004E-3</v>
-      </c>
       <c r="E36" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F36" s="1" t="e">
-        <f>(C36-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G36" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F36-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F36" s="1">
+        <v>38.81</v>
+      </c>
+      <c r="G36" s="16">
+        <v>1.6040000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3471,23 +3392,14 @@
       <c r="B37" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C37">
-        <v>0.11</v>
-      </c>
-      <c r="D37">
-        <f>2.1/100*C37</f>
-        <v>2.31E-3</v>
-      </c>
       <c r="E37" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="1" t="e">
-        <f>(C37-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G37" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F37-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F37" s="1">
+        <v>38.840000000000003</v>
+      </c>
+      <c r="G37" s="16">
+        <v>1.5049999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3497,23 +3409,14 @@
       <c r="B38" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C38">
-        <v>0.11</v>
-      </c>
-      <c r="D38">
-        <f>C38*0.023</f>
-        <v>2.5300000000000001E-3</v>
-      </c>
       <c r="E38" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F38" s="1" t="e">
-        <f>(C38-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G38" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F38-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F38" s="1">
+        <v>40.43</v>
+      </c>
+      <c r="G38" s="16">
+        <v>1.591</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3523,23 +3426,14 @@
       <c r="B39" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C39">
-        <v>0.53</v>
-      </c>
-      <c r="D39">
-        <f>0.01*C39</f>
-        <v>5.3E-3</v>
-      </c>
       <c r="E39" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F39" s="1" t="e">
-        <f>(C39-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G39" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F39-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F39" s="1">
+        <v>192.2</v>
+      </c>
+      <c r="G39" s="16">
+        <v>6.4370000000000003</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3549,23 +3443,14 @@
       <c r="B40" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C40">
-        <v>0.49</v>
-      </c>
-      <c r="D40">
-        <f>C40*0.013</f>
-        <v>6.3699999999999998E-3</v>
-      </c>
       <c r="E40" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F40" s="1" t="e">
-        <f>(C40-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G40" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F40-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F40" s="1">
+        <v>181.3</v>
+      </c>
+      <c r="G40" s="16">
+        <v>6.2560000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3575,23 +3460,14 @@
       <c r="B41" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C41">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D41">
-        <f>0.04*C41</f>
-        <v>2.2000000000000002E-2</v>
-      </c>
       <c r="E41" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F41" s="1" t="e">
-        <f>(C41-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G41" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F41-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
+      <c r="F41" s="1">
+        <v>197.3</v>
+      </c>
+      <c r="G41" s="16">
+        <v>10.15</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3601,24 +3477,13 @@
       <c r="B42" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="15">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D42" s="15">
-        <f>0.213*C42</f>
-        <v>8.52E-4</v>
-      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
       <c r="E42" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F42" s="1" t="e">
-        <f>(C42-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G42" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F42-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
@@ -3627,24 +3492,13 @@
       <c r="B43" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="15">
-        <v>5.8999999999999999E-3</v>
-      </c>
-      <c r="D43" s="15">
-        <f>0.127*C43</f>
-        <v>7.4929999999999994E-4</v>
-      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
       <c r="E43" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F43" s="1" t="e">
-        <f>(C43-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G43" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F43-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
@@ -3653,24 +3507,11 @@
       <c r="B44" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C44">
-        <v>0.48</v>
-      </c>
-      <c r="D44">
-        <f>C44*0.012</f>
-        <v>5.7599999999999995E-3</v>
-      </c>
       <c r="E44" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F44" s="1" t="e">
-        <f>(C44-'Calibration Data'!$L$64)/'Calibration Data'!$L$65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G44" s="16" t="e">
-        <f>'Calibration Data'!$L$54/'Calibration Data'!$L$65*SQRT(1/'Calibration Data'!$L$55+1+('Count-&gt;Actual Activity'!F44-AVERAGE('Calibration Data'!$F$3:$F$8))^2/('Calibration Data'!$L$65^2*'Calibration Data'!$J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3682,7 +3523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -6386,10 +6227,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6532,31 +6376,37 @@
       <c r="H2" s="1">
         <v>5</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="1">
+        <f>'Count-&gt;Actual Activity'!F2</f>
+        <v>0.13863585962890326</v>
+      </c>
+      <c r="J2" s="1">
+        <f>'Count-&gt;Actual Activity'!G2</f>
+        <v>0.1266475721979699</v>
+      </c>
       <c r="K2">
         <v>10</v>
       </c>
       <c r="L2">
         <v>0.02</v>
       </c>
-      <c r="M2" s="1" t="e">
+      <c r="M2" s="1">
         <f>'Count-&gt;Actual Activity'!F24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N2" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
         <f>'Count-&gt;Actual Activity'!G24</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2">
         <f>I2/K2</f>
-        <v>0</v>
-      </c>
-      <c r="R2" t="e">
+        <v>1.3863585962890326E-2</v>
+      </c>
+      <c r="R2">
         <f>Q2*SQRT((J2/I2)^2+(L2/K2)^2)</f>
-        <v>#DIV/0!</v>
+        <v>1.2664787571549038E-2</v>
       </c>
       <c r="S2" t="e">
         <f>M2/O2</f>
@@ -6576,14 +6426,14 @@
       </c>
       <c r="W2">
         <f>Q2</f>
-        <v>0</v>
+        <v>1.3863585962890326E-2</v>
       </c>
       <c r="X2">
         <v>2.3297918868665893E-2</v>
       </c>
       <c r="Y2">
         <f>(U2-Q2*G2)/E2</f>
-        <v>0</v>
+        <v>-46.211953209634423</v>
       </c>
       <c r="AA2" t="s">
         <v>123</v>
@@ -6618,31 +6468,37 @@
       <c r="H3" s="1">
         <v>5</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="1">
+        <f>'Count-&gt;Actual Activity'!F3</f>
+        <v>0.14271465019157553</v>
+      </c>
+      <c r="J3" s="1">
+        <f>'Count-&gt;Actual Activity'!G3</f>
+        <v>0.12664753145957777</v>
+      </c>
       <c r="K3">
         <v>10</v>
       </c>
       <c r="L3">
         <v>0.02</v>
       </c>
-      <c r="M3" s="1" t="e">
+      <c r="M3" s="1">
         <f>'Count-&gt;Actual Activity'!F25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N3" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
         <f>'Count-&gt;Actual Activity'!G25</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3">
         <f t="shared" ref="Q3:Q23" si="0">I3/K3</f>
-        <v>0</v>
-      </c>
-      <c r="R3" t="e">
+        <v>1.4271465019157553E-2</v>
+      </c>
+      <c r="R3">
         <f t="shared" ref="R3:R23" si="1">Q3*SQRT((J3/I3)^2+(L3/K3)^2)</f>
-        <v>#DIV/0!</v>
+        <v>1.2664785309941206E-2</v>
       </c>
       <c r="S3" t="e">
         <f t="shared" ref="S3:S20" si="2">M3/O3</f>
@@ -6662,14 +6518,14 @@
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W23" si="4">Q3</f>
-        <v>0</v>
+        <v>1.4271465019157553E-2</v>
       </c>
       <c r="X3">
         <v>2.3297922254460427E-2</v>
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y7" si="5">(U3-Q3*G3)/E3</f>
-        <v>0</v>
+        <v>-47.57155006385851</v>
       </c>
       <c r="AA3" t="s">
         <v>123</v>
@@ -6704,31 +6560,37 @@
       <c r="H4" s="1">
         <v>5</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="1">
+        <f>'Count-&gt;Actual Activity'!F4</f>
+        <v>0.13435970823255169</v>
+      </c>
+      <c r="J4" s="1">
+        <f>'Count-&gt;Actual Activity'!G4</f>
+        <v>0.12664761490896947</v>
+      </c>
       <c r="K4">
         <v>10</v>
       </c>
       <c r="L4">
         <v>0.02</v>
       </c>
-      <c r="M4" s="1" t="e">
+      <c r="M4" s="1">
         <f>'Count-&gt;Actual Activity'!F26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N4" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
         <f>'Count-&gt;Actual Activity'!G26</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R4" t="e">
+        <v>1.3435970823255169E-2</v>
+      </c>
+      <c r="R4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.2664789999149379E-2</v>
       </c>
       <c r="S4" t="e">
         <f t="shared" si="2"/>
@@ -6748,14 +6610,14 @@
       </c>
       <c r="W4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.3435970823255169E-2</v>
       </c>
       <c r="X4">
         <v>2.3297915424772112E-2</v>
       </c>
       <c r="Y4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-44.786569410850568</v>
       </c>
       <c r="AA4" t="s">
         <v>123</v>
@@ -6790,39 +6652,47 @@
       <c r="H5" s="1">
         <v>5</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="I5" s="1">
+        <f>'Count-&gt;Actual Activity'!F5</f>
+        <v>0.13482021684446649</v>
+      </c>
+      <c r="J5" s="1">
+        <f>'Count-&gt;Actual Activity'!G5</f>
+        <v>0.12664761030925478</v>
+      </c>
       <c r="K5">
         <v>10</v>
       </c>
       <c r="L5">
         <v>0.02</v>
       </c>
-      <c r="M5" s="1" t="e">
+      <c r="M5" s="1">
         <f>'Count-&gt;Actual Activity'!F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N5" s="1" t="e">
+        <v>2.7749999999999999</v>
+      </c>
+      <c r="N5" s="1">
         <f>'Count-&gt;Actual Activity'!G27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O5" s="1"/>
+        <v>0.25219999999999998</v>
+      </c>
+      <c r="O5" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R5" t="e">
+        <v>1.3482021684446649E-2</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S5" t="e">
+        <v>1.2664789734933755E-2</v>
+      </c>
+      <c r="S5">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T5" t="e">
+        <v>126.13636363636364</v>
+      </c>
+      <c r="T5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>11.463636363636363</v>
       </c>
       <c r="U5">
         <f>Parameters!$B$6*'Bottle Results'!B5</f>
@@ -6832,23 +6702,23 @@
         <f>SQRT((C5/B5)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>0.12773550438019637</v>
       </c>
-      <c r="W5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="W5" s="23">
+        <f>(U5-S5*O5)/G5</f>
+        <v>-6.8764827081244648E-4</v>
       </c>
       <c r="X5">
         <v>2.3297915790452959E-2</v>
       </c>
       <c r="Y5">
         <f t="shared" si="5"/>
-        <v>90.207839097291838</v>
+        <v>45.267766815803007</v>
       </c>
       <c r="AA5" t="s">
         <v>123</v>
       </c>
       <c r="AB5">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.50181633069583198</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -6876,39 +6746,47 @@
       <c r="H6" s="1">
         <v>5</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="I6" s="1">
+        <f>'Count-&gt;Actual Activity'!F6</f>
+        <v>0.13916215518537664</v>
+      </c>
+      <c r="J6" s="1">
+        <f>'Count-&gt;Actual Activity'!G6</f>
+        <v>0.1266475669413302</v>
+      </c>
       <c r="K6">
         <v>10</v>
       </c>
       <c r="L6">
         <v>0.02</v>
       </c>
-      <c r="M6" s="1" t="e">
+      <c r="M6" s="1">
         <f>'Count-&gt;Actual Activity'!F28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N6" s="1" t="e">
+        <v>3.2250000000000001</v>
+      </c>
+      <c r="N6" s="1">
         <f>'Count-&gt;Actual Activity'!G28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="1"/>
+        <v>0.2591</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6" t="e">
+        <v>1.3916215518537663E-2</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" t="e">
+        <v>1.2664787276768787E-2</v>
+      </c>
+      <c r="S6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T6" t="e">
+        <v>146.59090909090909</v>
+      </c>
+      <c r="T6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>11.777272727272726</v>
       </c>
       <c r="U6">
         <f>Parameters!$B$6*'Bottle Results'!B6</f>
@@ -6918,23 +6796,23 @@
         <f>SQRT((C6/B6)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>0.12773550438019637</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="W6" s="23">
+        <f t="shared" ref="W6:W16" si="7">(U6-S6*O6)/G6</f>
+        <v>-5.1876482708124484E-3</v>
       </c>
       <c r="X6">
         <v>2.3297919300009583E-2</v>
       </c>
       <c r="Y6">
         <f t="shared" si="5"/>
-        <v>90.207839097291838</v>
+        <v>43.820454035499637</v>
       </c>
       <c r="AA6" t="s">
         <v>123</v>
       </c>
       <c r="AB6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.48577212883059939</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -6962,35 +6840,43 @@
       <c r="H7" s="1">
         <v>5</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="1">
+        <f>'Count-&gt;Actual Activity'!F7</f>
+        <v>0.13087300017091258</v>
+      </c>
+      <c r="J7" s="1">
+        <f>'Count-&gt;Actual Activity'!G7</f>
+        <v>0.12664764973591827</v>
+      </c>
       <c r="K7">
         <v>10</v>
       </c>
       <c r="L7">
         <v>0.02</v>
       </c>
-      <c r="M7" s="1" t="e">
+      <c r="M7" s="1">
         <f>'Count-&gt;Actual Activity'!F29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" s="1" t="e">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
         <f>'Count-&gt;Actual Activity'!G29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O7" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7">
         <f t="shared" si="0"/>
+        <v>1.3087300017091259E-2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>1.2664792021427172E-2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="R7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
       </c>
       <c r="T7" t="e">
         <f t="shared" si="3"/>
@@ -7004,23 +6890,23 @@
         <f>SQRT((C7/B7)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>0.12773550438019637</v>
       </c>
-      <c r="W7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="W7" s="23">
+        <f t="shared" si="7"/>
+        <v>2.7062351729187552E-2</v>
       </c>
       <c r="X7">
         <v>2.3297912696774961E-2</v>
       </c>
       <c r="Y7">
         <f t="shared" si="5"/>
-        <v>90.207839097291838</v>
+        <v>46.583505706987644</v>
       </c>
       <c r="AA7" t="s">
         <v>123</v>
       </c>
       <c r="AB7">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.51640196875513167</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7048,11 +6934,11 @@
       <c r="H8" s="24">
         <v>5</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="1">
         <f>'Count-&gt;Actual Activity'!F8</f>
         <v>0.13251767378489365</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="1">
         <f>'Count-&gt;Actual Activity'!G8</f>
         <v>0.12664763330799395</v>
       </c>
@@ -7062,16 +6948,16 @@
       <c r="L8" s="23">
         <v>0.02</v>
       </c>
-      <c r="M8" s="24" t="e">
+      <c r="M8" s="1">
         <f>'Count-&gt;Actual Activity'!F30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N8" s="24" t="e">
+        <v>6.1120000000000001</v>
+      </c>
+      <c r="N8" s="1">
         <f>'Count-&gt;Actual Activity'!G30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="23">
-        <v>0.03</v>
+        <v>0.32490000000000002</v>
+      </c>
+      <c r="O8" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P8" s="23">
         <v>9.0000000000000006E-5</v>
@@ -7084,13 +6970,13 @@
         <f t="shared" si="1"/>
         <v>1.2664791062726444E-2</v>
       </c>
-      <c r="S8" s="23" t="e">
+      <c r="S8" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T8" s="23" t="e">
+        <v>277.81818181818181</v>
+      </c>
+      <c r="T8" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>23.105142153086835</v>
       </c>
       <c r="U8" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B8</f>
@@ -7101,23 +6987,23 @@
         <v>6.6180636102176282E-2</v>
       </c>
       <c r="W8" s="23">
-        <f t="shared" si="4"/>
-        <v>1.3251767378489366E-2</v>
+        <f t="shared" si="7"/>
+        <v>-7.1319750857116839E-3</v>
       </c>
       <c r="X8" s="23">
         <v>2.3297913974600508E-2</v>
       </c>
-      <c r="Y8" s="23" t="e">
-        <f t="shared" ref="Y8:Y19" si="7">S8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA8" s="23" t="e">
-        <f>(Q8*G8+S8*O8-U8)/U8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB8" s="23" t="e">
+      <c r="Y8" s="23">
+        <f t="shared" ref="Y8:Y19" si="8">S8</f>
+        <v>277.81818181818181</v>
+      </c>
+      <c r="AA8" s="23">
+        <f>(Q8*G8+S8*E8-U8)/U8</f>
+        <v>0.78923422513237329</v>
+      </c>
+      <c r="AB8" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.5437766926605345</v>
       </c>
     </row>
     <row r="9" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7145,11 +7031,11 @@
       <c r="H9" s="24">
         <v>5</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="1">
         <f>'Count-&gt;Actual Activity'!F9</f>
         <v>0.13620174268021087</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="1">
         <f>'Count-&gt;Actual Activity'!G9</f>
         <v>0.12664759651021001</v>
       </c>
@@ -7159,16 +7045,16 @@
       <c r="L9" s="23">
         <v>0.02</v>
       </c>
-      <c r="M9" s="24" t="e">
+      <c r="M9" s="1">
         <f>'Count-&gt;Actual Activity'!F31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="24" t="e">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="N9" s="1">
         <f>'Count-&gt;Actual Activity'!G31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="23">
-        <v>0.03</v>
+        <v>0.3201</v>
+      </c>
+      <c r="O9" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P9" s="23">
         <v>9.0000000000000006E-5</v>
@@ -7181,13 +7067,13 @@
         <f t="shared" si="1"/>
         <v>1.2664788946315605E-2</v>
       </c>
-      <c r="S9" s="23" t="e">
+      <c r="S9" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T9" s="23" t="e">
+        <v>272.63636363636368</v>
+      </c>
+      <c r="T9" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>22.710838231515403</v>
       </c>
       <c r="U9" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B9</f>
@@ -7198,23 +7084,23 @@
         <v>6.6180636102176282E-2</v>
       </c>
       <c r="W9" s="23">
-        <f t="shared" si="4"/>
-        <v>1.3620174268021087E-2</v>
+        <f t="shared" si="7"/>
+        <v>-5.9919750857117026E-3</v>
       </c>
       <c r="X9" s="23">
         <v>2.3297916895026565E-2</v>
       </c>
-      <c r="Y9" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA9" s="23" t="e">
-        <f>(Q9*G9+S9*O9-U9)/U9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB9" s="23" t="e">
+      <c r="Y9" s="23">
+        <f t="shared" si="8"/>
+        <v>272.63636363636368</v>
+      </c>
+      <c r="AA9" s="23">
+        <f t="shared" ref="AA9:AA19" si="9">(Q9*G9+S9*E9-U9)/U9</f>
+        <v>0.76726382397587889</v>
+      </c>
+      <c r="AB9" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.514982428432246</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7242,11 +7128,11 @@
       <c r="H10" s="24">
         <v>5</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="1">
         <f>'Count-&gt;Actual Activity'!F10</f>
         <v>0.1394910899081731</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="1">
         <f>'Count-&gt;Actual Activity'!G10</f>
         <v>0.12664756365594135</v>
       </c>
@@ -7256,16 +7142,16 @@
       <c r="L10" s="23">
         <v>0.02</v>
       </c>
-      <c r="M10" s="24" t="e">
+      <c r="M10" s="1">
         <f>'Count-&gt;Actual Activity'!F32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" s="24" t="e">
+        <v>5.6020000000000003</v>
+      </c>
+      <c r="N10" s="1">
         <f>'Count-&gt;Actual Activity'!G32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O10" s="23">
-        <v>0.03</v>
+        <v>0.37659999999999999</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P10" s="23">
         <v>9.0000000000000006E-5</v>
@@ -7278,13 +7164,13 @@
         <f t="shared" si="1"/>
         <v>1.2664787092976483E-2</v>
       </c>
-      <c r="S10" s="23" t="e">
+      <c r="S10" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T10" s="23" t="e">
+        <v>254.63636363636365</v>
+      </c>
+      <c r="T10" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>23.628063307376685</v>
       </c>
       <c r="U10" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B10</f>
@@ -7295,23 +7181,23 @@
         <v>6.6180636102176282E-2</v>
       </c>
       <c r="W10" s="23">
-        <f t="shared" si="4"/>
-        <v>1.394910899081731E-2</v>
+        <f t="shared" si="7"/>
+        <v>-2.0319750857116948E-3</v>
       </c>
       <c r="X10" s="23">
         <v>2.3297919570431896E-2</v>
       </c>
-      <c r="Y10" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA10" s="23" t="e">
-        <f>(Q10*G10+S10*O10-U10)/U10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB10" s="23" t="e">
+      <c r="Y10" s="23">
+        <f t="shared" si="8"/>
+        <v>254.63636363636365</v>
+      </c>
+      <c r="AA10" s="23">
+        <f t="shared" si="9"/>
+        <v>0.67333437785788086</v>
+      </c>
+      <c r="AB10" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.4149602474287164</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7339,41 +7225,47 @@
       <c r="H11" s="24">
         <v>5</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
+      <c r="I11" s="1">
+        <f>'Count-&gt;Actual Activity'!F11</f>
+        <v>0.13909636824081686</v>
+      </c>
+      <c r="J11" s="1">
+        <f>'Count-&gt;Actual Activity'!G11</f>
+        <v>0.12664756759840898</v>
+      </c>
       <c r="K11" s="23">
         <v>10</v>
       </c>
       <c r="L11" s="23">
         <v>0.02</v>
       </c>
-      <c r="M11" s="24" t="e">
+      <c r="M11" s="1">
         <f>'Count-&gt;Actual Activity'!F33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="24" t="e">
+        <v>21.28</v>
+      </c>
+      <c r="N11" s="1">
         <f>'Count-&gt;Actual Activity'!G33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O11" s="24">
-        <v>0.03</v>
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="O11" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P11" s="24"/>
       <c r="Q11" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="23" t="e">
+        <v>1.3909636824081686E-2</v>
+      </c>
+      <c r="R11" s="23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S11" s="23" t="e">
+        <v>1.2664787313568357E-2</v>
+      </c>
+      <c r="S11" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T11" s="23" t="e">
+        <v>967.27272727272737</v>
+      </c>
+      <c r="T11" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>47.772727272727273</v>
       </c>
       <c r="U11" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B11</f>
@@ -7383,23 +7275,24 @@
         <f>SQRT((C11/B11)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.1834127968683831E-2</v>
       </c>
-      <c r="W11" s="23" t="e">
-        <f t="shared" ref="W11:W19" si="8">(U11-S11*O11)/G11</f>
-        <v>#DIV/0!</v>
+      <c r="W11" s="23">
+        <f t="shared" si="7"/>
+        <v>5.7481820931658517E-2</v>
       </c>
       <c r="X11" s="23">
         <v>2.3297919246001962E-2</v>
       </c>
-      <c r="Y11" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA11" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB11" s="23" t="e">
+      <c r="Y11" s="23">
+        <f t="shared" si="8"/>
+        <v>967.27272727272737</v>
+      </c>
+      <c r="AA11" s="23">
+        <f t="shared" si="9"/>
+        <v>0.12509030003460803</v>
+      </c>
+      <c r="AB11" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.0736268432022715</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7427,41 +7320,47 @@
       <c r="H12" s="24">
         <v>5</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
+      <c r="I12" s="1">
+        <f>'Count-&gt;Actual Activity'!F12</f>
+        <v>0.13718854684859907</v>
+      </c>
+      <c r="J12" s="1">
+        <f>'Count-&gt;Actual Activity'!G12</f>
+        <v>0.12664758665384068</v>
+      </c>
       <c r="K12" s="23">
         <v>10</v>
       </c>
       <c r="L12" s="23">
         <v>0.02</v>
       </c>
-      <c r="M12" s="24" t="e">
+      <c r="M12" s="1">
         <f>'Count-&gt;Actual Activity'!F34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" s="24" t="e">
+        <v>20.83</v>
+      </c>
+      <c r="N12" s="1">
         <f>'Count-&gt;Actual Activity'!G34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O12" s="24">
-        <v>0.03</v>
+        <v>0.94069999999999998</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P12" s="24"/>
       <c r="Q12" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="23" t="e">
+        <v>1.3718854684859907E-2</v>
+      </c>
+      <c r="R12" s="23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S12" s="23" t="e">
+        <v>1.2664788386716783E-2</v>
+      </c>
+      <c r="S12" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T12" s="23" t="e">
+        <v>946.81818181818176</v>
+      </c>
+      <c r="T12" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>42.759090909090908</v>
       </c>
       <c r="U12" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B12</f>
@@ -7471,23 +7370,24 @@
         <f>SQRT((C12/B12)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.1834127968683831E-2</v>
       </c>
-      <c r="W12" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W12" s="23">
+        <f t="shared" si="7"/>
+        <v>6.1981820931658549E-2</v>
       </c>
       <c r="X12" s="23">
         <v>2.3297917690924E-2</v>
       </c>
-      <c r="Y12" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA12" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB12" s="23" t="e">
+      <c r="Y12" s="23">
+        <f t="shared" si="8"/>
+        <v>946.81818181818176</v>
+      </c>
+      <c r="AA12" s="23">
+        <f t="shared" si="9"/>
+        <v>0.10168086112459977</v>
+      </c>
+      <c r="AB12" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.0509232680405693</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7515,41 +7415,47 @@
       <c r="H13" s="24">
         <v>5</v>
       </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
+      <c r="I13" s="1">
+        <f>'Count-&gt;Actual Activity'!F13</f>
+        <v>0.14014895935376481</v>
+      </c>
+      <c r="J13" s="1">
+        <f>'Count-&gt;Actual Activity'!G13</f>
+        <v>0.12664755708518899</v>
+      </c>
       <c r="K13" s="23">
         <v>10</v>
       </c>
       <c r="L13" s="23">
         <v>0.02</v>
       </c>
-      <c r="M13" s="24" t="e">
+      <c r="M13" s="1">
         <f>'Count-&gt;Actual Activity'!F35</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" s="24" t="e">
+        <v>21.45</v>
+      </c>
+      <c r="N13" s="1">
         <f>'Count-&gt;Actual Activity'!G35</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O13" s="24">
-        <v>0.03</v>
+        <v>1.032</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P13" s="24"/>
       <c r="Q13" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="23" t="e">
+        <v>1.4014895935376481E-2</v>
+      </c>
+      <c r="R13" s="23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" s="23" t="e">
+        <v>1.2664786726419609E-2</v>
+      </c>
+      <c r="S13" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T13" s="23" t="e">
+        <v>975</v>
+      </c>
+      <c r="T13" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>46.909090909090914</v>
       </c>
       <c r="U13" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B13</f>
@@ -7559,23 +7465,24 @@
         <f>SQRT((C13/B13)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>3.1834127968683831E-2</v>
       </c>
-      <c r="W13" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W13" s="23">
+        <f t="shared" si="7"/>
+        <v>5.5781820931658538E-2</v>
       </c>
       <c r="X13" s="23">
         <v>2.3297920113197729E-2</v>
       </c>
-      <c r="Y13" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA13" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB13" s="23" t="e">
+      <c r="Y13" s="23">
+        <f t="shared" si="8"/>
+        <v>975</v>
+      </c>
+      <c r="AA13" s="23">
+        <f t="shared" si="9"/>
+        <v>0.13405664827483743</v>
+      </c>
+      <c r="AB13" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.0822037493744701</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7603,11 +7510,11 @@
       <c r="H14" s="24">
         <v>5</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="1">
         <f>'Count-&gt;Actual Activity'!F14</f>
         <v>0.14685922769880755</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="1">
         <f>'Count-&gt;Actual Activity'!G14</f>
         <v>0.12664749006544551</v>
       </c>
@@ -7617,16 +7524,16 @@
       <c r="L14" s="23">
         <v>0.02</v>
       </c>
-      <c r="M14" s="24" t="e">
+      <c r="M14" s="1">
         <f>'Count-&gt;Actual Activity'!F36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" s="24" t="e">
+        <v>38.81</v>
+      </c>
+      <c r="N14" s="1">
         <f>'Count-&gt;Actual Activity'!G36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O14" s="24">
-        <v>0.03</v>
+        <v>1.6040000000000001</v>
+      </c>
+      <c r="O14" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P14" s="24"/>
       <c r="Q14" s="23">
@@ -7637,13 +7544,13 @@
         <f t="shared" si="1"/>
         <v>1.2664783065812127E-2</v>
       </c>
-      <c r="S14" s="23" t="e">
+      <c r="S14" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T14" s="23" t="e">
+        <v>1764.0909090909092</v>
+      </c>
+      <c r="T14" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>72.909090909090907</v>
       </c>
       <c r="U14" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B14</f>
@@ -7653,24 +7560,24 @@
         <f>SQRT((C14/B14)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>2.3115774284716652E-2</v>
       </c>
-      <c r="W14" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W14" s="23">
+        <f t="shared" si="7"/>
+        <v>0.15178024914288302</v>
       </c>
       <c r="X14" s="23">
         <v>2.3297925795726985E-2</v>
       </c>
-      <c r="Y14" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA14" s="23" t="e">
-        <f>(Q14*G14+S14*O14-U14)/U14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB14" s="23" t="e">
+      <c r="Y14" s="23">
+        <f t="shared" si="8"/>
+        <v>1764.0909090909092</v>
+      </c>
+      <c r="AA14" s="23">
+        <f t="shared" si="9"/>
+        <v>7.4700757448956118E-3</v>
+      </c>
+      <c r="AB14" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>0.98026789008762027</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7698,41 +7605,47 @@
       <c r="H15" s="24">
         <v>5</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
+      <c r="I15" s="1">
+        <f>'Count-&gt;Actual Activity'!F15</f>
+        <v>0.14863547520190695</v>
+      </c>
+      <c r="J15" s="1">
+        <f>'Count-&gt;Actual Activity'!G15</f>
+        <v>0.12664747232551371</v>
+      </c>
       <c r="K15" s="23">
         <v>10</v>
       </c>
       <c r="L15" s="23">
         <v>0.02</v>
       </c>
-      <c r="M15" s="24" t="e">
+      <c r="M15" s="1">
         <f>'Count-&gt;Actual Activity'!F37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" s="24" t="e">
+        <v>38.840000000000003</v>
+      </c>
+      <c r="N15" s="1">
         <f>'Count-&gt;Actual Activity'!G37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="24">
-        <v>0.03</v>
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P15" s="24"/>
       <c r="Q15" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="23" t="e">
+        <v>1.4863547520190696E-2</v>
+      </c>
+      <c r="R15" s="23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S15" s="23" t="e">
+        <v>1.2664782120691899E-2</v>
+      </c>
+      <c r="S15" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T15" s="23" t="e">
+        <v>1765.4545454545457</v>
+      </c>
+      <c r="T15" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>68.409090909090907</v>
       </c>
       <c r="U15" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B15</f>
@@ -7742,24 +7655,24 @@
         <f>SQRT((C15/B15)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>2.3115774284716652E-2</v>
       </c>
-      <c r="W15" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W15" s="23">
+        <f t="shared" si="7"/>
+        <v>0.15148024914288299</v>
       </c>
       <c r="X15" s="23">
         <v>2.329792734453592E-2</v>
       </c>
-      <c r="Y15" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA15" s="23" t="e">
-        <f>(Q15*G15+S15*O15-U15)/U15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB15" s="23" t="e">
+      <c r="Y15" s="23">
+        <f t="shared" si="8"/>
+        <v>1765.4545454545457</v>
+      </c>
+      <c r="AA15" s="23">
+        <f t="shared" si="9"/>
+        <v>8.5568272241956112E-3</v>
+      </c>
+      <c r="AB15" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>0.98102563388310171</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -7787,41 +7700,47 @@
       <c r="H16" s="24">
         <v>5</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="I16" s="1">
+        <f>'Count-&gt;Actual Activity'!F16</f>
+        <v>0.15166167465163247</v>
+      </c>
+      <c r="J16" s="1">
+        <f>'Count-&gt;Actual Activity'!G16</f>
+        <v>0.12664744210249368</v>
+      </c>
       <c r="K16" s="23">
         <v>10</v>
       </c>
       <c r="L16" s="23">
         <v>0.02</v>
       </c>
-      <c r="M16" s="24" t="e">
+      <c r="M16" s="1">
         <f>'Count-&gt;Actual Activity'!F38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="24" t="e">
+        <v>40.43</v>
+      </c>
+      <c r="N16" s="1">
         <f>'Count-&gt;Actual Activity'!G38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="24">
-        <v>0.03</v>
+        <v>1.591</v>
+      </c>
+      <c r="O16" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P16" s="24"/>
       <c r="Q16" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="23" t="e">
+        <v>1.5166167465163246E-2</v>
+      </c>
+      <c r="R16" s="23">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S16" s="23" t="e">
+        <v>1.2664780533494735E-2</v>
+      </c>
+      <c r="S16" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T16" s="23" t="e">
+        <v>1837.7272727272727</v>
+      </c>
+      <c r="T16" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>72.318181818181827</v>
       </c>
       <c r="U16" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B16</f>
@@ -7831,27 +7750,28 @@
         <f>SQRT((C16/B16)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>2.3115774284716652E-2</v>
       </c>
-      <c r="W16" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W16" s="23">
+        <f t="shared" si="7"/>
+        <v>0.13558024914288302</v>
       </c>
       <c r="X16" s="23">
         <v>2.3297930026256426E-2</v>
       </c>
-      <c r="Y16" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="Y16" s="23">
+        <f t="shared" si="8"/>
+        <v>1837.7272727272727</v>
       </c>
       <c r="Z16" s="23"/>
-      <c r="AA16" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB16" s="23" t="e">
+      <c r="AA16" s="23">
+        <f t="shared" si="9"/>
+        <v>4.9277779994172571E-2</v>
+      </c>
+      <c r="AB16" s="23">
         <f>Y16*E16/U16</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1.0211860550436096</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>103</v>
       </c>
@@ -7876,11 +7796,11 @@
       <c r="H17" s="24">
         <v>5</v>
       </c>
-      <c r="I17" s="24">
+      <c r="I17" s="1">
         <f>'Count-&gt;Actual Activity'!F17</f>
         <v>0.35829846751220068</v>
       </c>
-      <c r="J17" s="24">
+      <c r="J17" s="1">
         <f>'Count-&gt;Actual Activity'!G17</f>
         <v>0.12664538008742116</v>
       </c>
@@ -7890,16 +7810,16 @@
       <c r="L17" s="23">
         <v>0.02</v>
       </c>
-      <c r="M17" s="24" t="e">
+      <c r="M17" s="1">
         <f>'Count-&gt;Actual Activity'!F39</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N17" s="24" t="e">
+        <v>192.2</v>
+      </c>
+      <c r="N17" s="1">
         <f>'Count-&gt;Actual Activity'!G39</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="23">
-        <v>0.03</v>
+        <v>6.4370000000000003</v>
+      </c>
+      <c r="O17" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P17" s="23">
         <v>9.0000000000000006E-5</v>
@@ -7912,13 +7832,13 @@
         <f t="shared" si="1"/>
         <v>1.2664740742966144E-2</v>
       </c>
-      <c r="S17" s="23" t="e">
+      <c r="S17" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T17" s="23" t="e">
+        <v>8736.363636363636</v>
+      </c>
+      <c r="T17" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>630.7489107340466</v>
       </c>
       <c r="U17" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B17</f>
@@ -7928,30 +7848,34 @@
         <f>SQRT((C17/B17)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>1.9506029550982833E-2</v>
       </c>
-      <c r="W17" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W17" s="23">
+        <f>Q17</f>
+        <v>3.5829846751220071E-2</v>
       </c>
       <c r="X17" s="23">
         <v>2.3298241351735846E-2</v>
       </c>
-      <c r="Y17" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="Y17" s="23">
+        <f t="shared" si="8"/>
+        <v>8736.363636363636</v>
       </c>
       <c r="Z17" s="23">
         <v>750.18565608355891</v>
       </c>
-      <c r="AA17" s="23" t="e">
-        <f>(Q17*G17+S17*O17-U17)/U17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB17" s="23" t="e">
+      <c r="AA17" s="23">
+        <f t="shared" si="9"/>
+        <v>-1.8289702149226528E-2</v>
+      </c>
+      <c r="AB17" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.96847055907649071</v>
+      </c>
+      <c r="AC17" s="23">
+        <f>(U17-Q17*G17)/U17</f>
+        <v>0.98676026122571725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>104</v>
       </c>
@@ -7976,11 +7900,11 @@
       <c r="H18" s="24">
         <v>5</v>
       </c>
-      <c r="I18" s="24">
+      <c r="I18" s="1">
         <f>'Count-&gt;Actual Activity'!F18</f>
         <v>0.29856392185241143</v>
       </c>
-      <c r="J18" s="24">
+      <c r="J18" s="1">
         <f>'Count-&gt;Actual Activity'!G18</f>
         <v>0.1266459758319273</v>
       </c>
@@ -7990,16 +7914,16 @@
       <c r="L18" s="23">
         <v>0.02</v>
       </c>
-      <c r="M18" s="24" t="e">
+      <c r="M18" s="1">
         <f>'Count-&gt;Actual Activity'!F40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="24" t="e">
+        <v>181.3</v>
+      </c>
+      <c r="N18" s="1">
         <f>'Count-&gt;Actual Activity'!G40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="23">
-        <v>0.03</v>
+        <v>6.2560000000000002</v>
+      </c>
+      <c r="O18" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P18" s="23">
         <v>9.0000000000000006E-5</v>
@@ -8012,13 +7936,13 @@
         <f t="shared" si="1"/>
         <v>1.2664738353429511E-2</v>
       </c>
-      <c r="S18" s="23" t="e">
+      <c r="S18" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T18" s="23" t="e">
+        <v>8240.9090909090919</v>
+      </c>
+      <c r="T18" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>598.90473317045542</v>
       </c>
       <c r="U18" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B18</f>
@@ -8028,30 +7952,34 @@
         <f>SQRT((C18/B18)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>1.9506029550982833E-2</v>
       </c>
-      <c r="W18" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W18" s="23">
+        <f>Q18</f>
+        <v>2.9856392185241144E-2</v>
       </c>
       <c r="X18" s="23">
         <v>2.3298125385430756E-2</v>
       </c>
-      <c r="Y18" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="Y18" s="23">
+        <f t="shared" si="8"/>
+        <v>8240.9090909090919</v>
       </c>
       <c r="Z18" s="23">
         <v>696.13408835057783</v>
       </c>
-      <c r="AA18" s="23" t="e">
-        <f>(Q18*G18+S18*O18-U18)/U18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB18" s="23" t="e">
+      <c r="AA18" s="23">
+        <f t="shared" si="9"/>
+        <v>-7.5420663918373487E-2</v>
+      </c>
+      <c r="AB18" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.91354689053365146</v>
+      </c>
+      <c r="AC18" s="23">
+        <f>(U18-Q18*G18)/U18</f>
+        <v>0.98896755445202489</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>105</v>
       </c>
@@ -8076,11 +8004,11 @@
       <c r="H19" s="24">
         <v>5</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="1">
         <f>'Count-&gt;Actual Activity'!F19</f>
         <v>0.2969192482384303</v>
       </c>
-      <c r="J19" s="24">
+      <c r="J19" s="1">
         <f>'Count-&gt;Actual Activity'!G19</f>
         <v>0.12664599223852602</v>
       </c>
@@ -8090,16 +8018,16 @@
       <c r="L19" s="23">
         <v>0.02</v>
       </c>
-      <c r="M19" s="24" t="e">
+      <c r="M19" s="1">
         <f>'Count-&gt;Actual Activity'!F41</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" s="24" t="e">
+        <v>197.3</v>
+      </c>
+      <c r="N19" s="1">
         <f>'Count-&gt;Actual Activity'!G41</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O19" s="23">
-        <v>0.03</v>
+        <v>10.15</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P19" s="23">
         <v>9.0000000000000006E-5</v>
@@ -8112,13 +8040,13 @@
         <f t="shared" si="1"/>
         <v>1.2664738447453501E-2</v>
       </c>
-      <c r="S19" s="23" t="e">
+      <c r="S19" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T19" s="23" t="e">
+        <v>8968.1818181818198</v>
+      </c>
+      <c r="T19" s="23">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>736.12580972177761</v>
       </c>
       <c r="U19" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B19</f>
@@ -8128,27 +8056,31 @@
         <f>SQRT((C19/B19)^2+(Parameters!$C$6/Parameters!$B$6))</f>
         <v>1.9506029550982833E-2</v>
       </c>
-      <c r="W19" s="23" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="W19" s="23">
+        <f>Q19</f>
+        <v>2.969192482384303E-2</v>
       </c>
       <c r="X19" s="23">
         <v>2.3298122491261654E-2</v>
       </c>
-      <c r="Y19" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA19" s="23" t="e">
-        <f>(Q19*G19+S19*O19-U19)/U19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB19" s="23" t="e">
+      <c r="Y19" s="23">
+        <f t="shared" si="8"/>
+        <v>8968.1818181818198</v>
+      </c>
+      <c r="AA19" s="23">
+        <f t="shared" si="9"/>
+        <v>5.1404613681927105E-3</v>
+      </c>
+      <c r="AB19" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.99416878931213137</v>
+      </c>
+      <c r="AC19" s="23">
+        <f>(U19-Q19*G19)/U19</f>
+        <v>0.98902832794393869</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>114</v>
       </c>
@@ -8181,13 +8113,13 @@
       <c r="L20" s="28">
         <v>0.02</v>
       </c>
-      <c r="M20" s="29" t="e">
+      <c r="M20" s="1">
         <f>'Count-&gt;Actual Activity'!F42</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" s="29" t="e">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
         <f>'Count-&gt;Actual Activity'!G42</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="O20" s="28">
         <v>0.03</v>
@@ -8203,9 +8135,9 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S20" s="28" t="e">
+      <c r="S20" s="28">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T20" s="28" t="e">
         <f t="shared" si="3"/>
@@ -8235,7 +8167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>129</v>
       </c>
@@ -8264,15 +8196,24 @@
         <f>'Count-&gt;Actual Activity'!F20</f>
         <v>0.59185856743363718</v>
       </c>
-      <c r="J21" s="29"/>
+      <c r="J21" s="29">
+        <f>'Count-&gt;Actual Activity'!G20</f>
+        <v>0.12664305342085061</v>
+      </c>
       <c r="K21" s="28">
         <v>10</v>
       </c>
       <c r="L21" s="28">
         <v>0.02</v>
       </c>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="M21" s="1">
+        <f>'Count-&gt;Actual Activity'!F43</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f>'Count-&gt;Actual Activity'!G43</f>
+        <v>0</v>
+      </c>
       <c r="O21" s="28">
         <v>0.03</v>
       </c>
@@ -8285,7 +8226,7 @@
       </c>
       <c r="R21" s="28">
         <f t="shared" si="1"/>
-        <v>1.1837171348672744E-4</v>
+        <v>1.2664858532969012E-2</v>
       </c>
       <c r="U21" s="28">
         <f>Parameters!$B$6*'Bottle Results'!B21</f>
@@ -8311,7 +8252,7 @@
         <v>0.97812981763904494</v>
       </c>
     </row>
-    <row r="22" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>133</v>
       </c>
@@ -8344,13 +8285,13 @@
       <c r="L22" s="28">
         <v>0.02</v>
       </c>
-      <c r="M22" s="29" t="e">
+      <c r="M22" s="1">
         <f>'Count-&gt;Actual Activity'!F44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" s="29" t="e">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
         <f>'Count-&gt;Actual Activity'!G44</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="O22" s="28">
         <v>0.03</v>
@@ -8390,7 +8331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>134</v>
       </c>
@@ -8423,11 +8364,11 @@
       <c r="L23" s="28">
         <v>0.02</v>
       </c>
-      <c r="M23" s="29">
+      <c r="M23" s="1">
         <f>'Count-&gt;Actual Activity'!F45</f>
         <v>0</v>
       </c>
-      <c r="N23" s="29">
+      <c r="N23" s="1">
         <f>'Count-&gt;Actual Activity'!G45</f>
         <v>0</v>
       </c>
@@ -8479,7 +8420,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8524,19 +8465,19 @@
       </c>
       <c r="B2">
         <f>AVERAGE('Bottle Results'!W2:W4)</f>
-        <v>0</v>
+        <v>1.3857007268434349E-2</v>
       </c>
       <c r="C2">
         <f>_xlfn.STDEV.S('Bottle Results'!W2:W4)</f>
-        <v>0</v>
+        <v>4.1778594670261653E-4</v>
       </c>
       <c r="D2">
         <f>AVERAGE('Bottle Results'!Y2:Y4)</f>
-        <v>0</v>
+        <v>-46.190024228114503</v>
       </c>
       <c r="E2">
         <f>_xlfn.STDEV.S('Bottle Results'!Y2:Y4)</f>
-        <v>0</v>
+        <v>1.3926198223420532</v>
       </c>
       <c r="F2" t="e">
         <f>AVERAGE('Bottle Results'!AB2:AB4)</f>
@@ -8561,27 +8502,27 @@
       </c>
       <c r="B3">
         <f>AVERAGE('Bottle Results'!W5:W7)</f>
-        <v>0</v>
+        <v>7.0623517291875521E-3</v>
       </c>
       <c r="C3">
         <f>_xlfn.STDEV.S('Bottle Results'!W5:W7)</f>
-        <v>0</v>
+        <v>1.7466038474708571E-2</v>
       </c>
       <c r="D3">
         <f>AVERAGE('Bottle Results'!Y5:Y7)</f>
-        <v>90.207839097291824</v>
+        <v>45.223908852763429</v>
       </c>
       <c r="E3">
         <f>_xlfn.STDEV.S('Bottle Results'!Y5:Y7)</f>
-        <v>1.7404671430534633E-14</v>
+        <v>1.3820478557270199</v>
       </c>
       <c r="F3">
         <f>AVERAGE('Bottle Results'!AB5:AB7)</f>
-        <v>1</v>
+        <v>0.50133014276052101</v>
       </c>
       <c r="G3">
         <f>_xlfn.STDEV.S('Bottle Results'!AB5:AB7)</f>
-        <v>0</v>
+        <v>1.532070682057291E-2</v>
       </c>
       <c r="H3">
         <f>AVERAGE('Bottle Results'!D5:D7)</f>
@@ -8598,27 +8539,27 @@
       </c>
       <c r="B4">
         <f>AVERAGE('Bottle Results'!W8:W10)</f>
-        <v>1.3607016879109255E-2</v>
+        <v>-5.051975085711694E-3</v>
       </c>
       <c r="C4">
         <f>_xlfn.STDEV.S('Bottle Results'!W8:W10)</f>
-        <v>3.4885694594384543E-4</v>
-      </c>
-      <c r="D4" t="e">
+        <v>2.6767891213168031E-3</v>
+      </c>
+      <c r="D4">
         <f>AVERAGE('Bottle Results'!Y8:Y10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" t="e">
+        <v>268.36363636363637</v>
+      </c>
+      <c r="E4">
         <f>_xlfn.STDEV.S('Bottle Results'!Y8:Y10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" t="e">
+        <v>12.167223278712751</v>
+      </c>
+      <c r="F4">
         <f>AVERAGE('Bottle Results'!AB8:AB10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>1.4912397895071656</v>
+      </c>
+      <c r="G4">
         <f>_xlfn.STDEV.S('Bottle Results'!AB8:AB10)</f>
-        <v>#DIV/0!</v>
+        <v>6.7610678282986877E-2</v>
       </c>
       <c r="H4">
         <f>AVERAGE('Bottle Results'!D8:D10)</f>
@@ -8633,29 +8574,29 @@
       <c r="A5" s="14">
         <v>50</v>
       </c>
-      <c r="B5" t="e">
+      <c r="B5">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" t="e">
+        <v>5.8415154264991866E-2</v>
+      </c>
+      <c r="C5">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" t="e">
+        <v>3.2036437588054936E-3</v>
+      </c>
+      <c r="D5">
         <f>AVERAGE('Bottle Results'!Y11:Y13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" t="e">
+        <v>963.030303030303</v>
+      </c>
+      <c r="E5">
         <f>_xlfn.STDEV.S('Bottle Results'!Y11:Y13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" t="e">
+        <v>14.562017085479523</v>
+      </c>
+      <c r="F5">
         <f>AVERAGE('Bottle Results'!AB11:AB13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" t="e">
+        <v>1.0689179535391036</v>
+      </c>
+      <c r="G5">
         <f>_xlfn.STDEV.S('Bottle Results'!AB11:AB13)</f>
-        <v>#DIV/0!</v>
+        <v>1.6163148193190729E-2</v>
       </c>
       <c r="H5">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
@@ -8670,29 +8611,29 @@
       <c r="A6" s="14">
         <v>100</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>AVERAGE('Bottle Results'!W14:W16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
+        <v>0.14628024914288301</v>
+      </c>
+      <c r="C6">
         <f>_xlfn.STDEV.S('Bottle Results'!W14:W16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
+        <v>9.2676857952781171E-3</v>
+      </c>
+      <c r="D6">
         <f>AVERAGE('Bottle Results'!Y14:Y16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
+        <v>1789.0909090909092</v>
+      </c>
+      <c r="E6">
         <f>_xlfn.STDEV.S('Bottle Results'!Y14:Y16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" t="e">
+        <v>42.12584452399139</v>
+      </c>
+      <c r="F6">
         <f>AVERAGE('Bottle Results'!AB14:AB16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" t="e">
+        <v>0.99415985967144371</v>
+      </c>
+      <c r="G6">
         <f>_xlfn.STDEV.S('Bottle Results'!AB14:AB16)</f>
-        <v>#DIV/0!</v>
+        <v>2.3408438032806719E-2</v>
       </c>
       <c r="H6">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
@@ -8707,29 +8648,29 @@
       <c r="A7" s="14">
         <v>500</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7">
         <f>AVERAGE('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
+        <v>3.8641005125916991E-2</v>
+      </c>
+      <c r="C7">
         <f>_xlfn.STDEV.S('Bottle Results'!W17:W19,'Bottle Results'!W21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
+        <v>1.3991056693009167E-2</v>
+      </c>
+      <c r="D7">
         <f>AVERAGE('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
+        <v>8692.2380665097971</v>
+      </c>
+      <c r="E7">
         <f>_xlfn.STDEV.S('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" t="e">
+        <v>315.71028966780398</v>
+      </c>
+      <c r="F7">
         <f>AVERAGE('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>0.96357901414032965</v>
+      </c>
+      <c r="G7">
         <f>_xlfn.STDEV.S('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>#DIV/0!</v>
+        <v>3.499809914826809E-2</v>
       </c>
       <c r="H7">
         <f>AVERAGE('Bottle Results'!D17:D19,'Bottle Results'!D21)</f>

</xml_diff>

<commit_message>
Fit FHY with new data points, data tweaking needed
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH9/RaFHY_pH9_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -2598,7 +2598,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6246,11 +6246,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y21" sqref="Y21"/>
+      <selection pane="bottomRight" activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6534,7 +6534,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W19" si="4">(U3-Y3*E3)/G3</f>
+        <f t="shared" ref="W3:W16" si="4">(U3-Y3*E3)/G3</f>
         <v>1.4271465019157553E-2</v>
       </c>
       <c r="X3">
@@ -6692,7 +6692,7 @@
         <v>0.25219999999999998</v>
       </c>
       <c r="O5" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P5" s="1">
         <v>5.0000000000000001E-3</v>
@@ -6707,11 +6707,11 @@
       </c>
       <c r="S5">
         <f t="shared" si="2"/>
-        <v>123.33333333333333</v>
+        <v>122.78761061946904</v>
       </c>
       <c r="T5">
         <f t="shared" si="3"/>
-        <v>59.210523589170393</v>
+        <v>58.822652332348568</v>
       </c>
       <c r="U5">
         <f>Parameters!$B$6*'Bottle Results'!B5</f>
@@ -6723,21 +6723,21 @@
       </c>
       <c r="W5">
         <f t="shared" si="4"/>
-        <v>1.3482021684446651E-2</v>
+        <v>-9.7739314566531559E-3</v>
       </c>
       <c r="X5">
         <v>2.3297915790452959E-2</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="5"/>
-        <v>45.267766815803007</v>
+        <f>S5</f>
+        <v>122.78761061946904</v>
       </c>
       <c r="AA5" t="s">
         <v>123</v>
       </c>
       <c r="AB5">
         <f t="shared" si="6"/>
-        <v>0.50181633069583198</v>
+        <v>1.361163418259459</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -6788,7 +6788,7 @@
         <v>0.2591</v>
       </c>
       <c r="O6" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P6" s="1">
         <v>5.0000000000000001E-3</v>
@@ -6803,11 +6803,11 @@
       </c>
       <c r="S6">
         <f t="shared" si="2"/>
-        <v>143.33333333333334</v>
+        <v>142.6991150442478</v>
       </c>
       <c r="T6">
         <f t="shared" si="3"/>
-        <v>68.542250608792529</v>
+        <v>68.092098449580178</v>
       </c>
       <c r="U6">
         <f>Parameters!$B$6*'Bottle Results'!B6</f>
@@ -6819,21 +6819,21 @@
       </c>
       <c r="W6">
         <f t="shared" si="4"/>
-        <v>1.3916215518537662E-2</v>
+        <v>-1.5747382784086782E-2</v>
       </c>
       <c r="X6">
         <v>2.3297919300009583E-2</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="5"/>
-        <v>43.820454035499637</v>
+        <f>S6</f>
+        <v>142.6991150442478</v>
       </c>
       <c r="AA6" t="s">
         <v>123</v>
       </c>
       <c r="AB6">
         <f t="shared" si="6"/>
-        <v>0.48577212883059939</v>
+        <v>1.5818926212204523</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -6884,7 +6884,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P7" s="1">
         <v>5.0000000000000001E-3</v>
@@ -6915,21 +6915,21 @@
       </c>
       <c r="W7">
         <f t="shared" si="4"/>
-        <v>1.3087300017091259E-2</v>
+        <v>2.7062351729187552E-2</v>
       </c>
       <c r="X7">
         <v>2.3297912696774961E-2</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="5"/>
-        <v>46.583505706987644</v>
+        <f>S7</f>
+        <v>0</v>
       </c>
       <c r="AA7" t="s">
         <v>123</v>
       </c>
       <c r="AB7">
         <f t="shared" si="6"/>
-        <v>0.51640196875513167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6980,7 +6980,7 @@
         <v>0.32490000000000002</v>
       </c>
       <c r="O8" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P8" s="1">
         <v>5.0000000000000001E-3</v>
@@ -6995,11 +6995,11 @@
       </c>
       <c r="S8" s="23">
         <f t="shared" si="2"/>
-        <v>271.64444444444445</v>
+        <v>270.44247787610624</v>
       </c>
       <c r="T8" s="23">
         <f t="shared" si="3"/>
-        <v>128.86600741125633</v>
+        <v>128.0152206972073</v>
       </c>
       <c r="U8" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B8</f>
@@ -7011,22 +7011,22 @@
       </c>
       <c r="W8">
         <f t="shared" si="4"/>
-        <v>-2.750530841904502E-2</v>
+        <v>-2.7144718448543558E-2</v>
       </c>
       <c r="X8" s="23">
         <v>2.3297913974600508E-2</v>
       </c>
       <c r="Y8" s="23">
         <f t="shared" ref="Y8:Y19" si="7">S8</f>
-        <v>271.64444444444445</v>
+        <v>270.44247787610624</v>
       </c>
       <c r="AA8" s="23">
         <f>(Q8*G8+S8*E8-U8)/U8</f>
-        <v>0.75492807640658366</v>
+        <v>0.74824900320333276</v>
       </c>
       <c r="AB8" s="23">
         <f t="shared" si="6"/>
-        <v>1.5094705439347449</v>
+        <v>1.502791470731494</v>
       </c>
     </row>
     <row r="9" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7077,7 +7077,7 @@
         <v>0.3201</v>
       </c>
       <c r="O9" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P9" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7092,11 +7092,11 @@
       </c>
       <c r="S9" s="23">
         <f t="shared" si="2"/>
-        <v>266.57777777777778</v>
+        <v>265.39823008849561</v>
       </c>
       <c r="T9" s="23">
         <f t="shared" si="3"/>
-        <v>126.46870742066177</v>
+        <v>125.63377533701315</v>
       </c>
       <c r="U9" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B9</f>
@@ -7108,22 +7108,22 @@
       </c>
       <c r="W9">
         <f t="shared" si="4"/>
-        <v>-2.5985308419045026E-2</v>
+        <v>-2.5631444112260374E-2</v>
       </c>
       <c r="X9" s="23">
         <v>2.3297916895026565E-2</v>
       </c>
       <c r="Y9" s="23">
         <f t="shared" si="7"/>
-        <v>266.57777777777778</v>
+        <v>265.39823008849561</v>
       </c>
       <c r="AA9" s="23">
         <f t="shared" ref="AA9:AA19" si="8">(Q9*G9+S9*E9-U9)/U9</f>
-        <v>0.73359754778849562</v>
+        <v>0.7270430515396249</v>
       </c>
       <c r="AB9" s="23">
         <f>Y9*E9/U9</f>
-        <v>1.4813161522448626</v>
+        <v>1.4747616559959917</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7174,7 +7174,7 @@
         <v>0.37659999999999999</v>
       </c>
       <c r="O10" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P10" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7189,11 +7189,11 @@
       </c>
       <c r="S10" s="23">
         <f t="shared" si="2"/>
-        <v>248.97777777777779</v>
+        <v>247.87610619469029</v>
       </c>
       <c r="T10" s="23">
         <f t="shared" si="3"/>
-        <v>118.5567124013583</v>
+        <v>117.77591890366479</v>
       </c>
       <c r="U10" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B10</f>
@@ -7205,22 +7205,22 @@
       </c>
       <c r="W10">
         <f t="shared" si="4"/>
-        <v>-2.0705308419045023E-2</v>
+        <v>-2.0374806944118778E-2</v>
       </c>
       <c r="X10" s="23">
         <v>2.3297919570431896E-2</v>
       </c>
       <c r="Y10" s="23">
         <f t="shared" si="7"/>
-        <v>248.97777777777779</v>
+        <v>247.87610619469029</v>
       </c>
       <c r="AA10" s="23">
         <f t="shared" si="8"/>
-        <v>0.64189081680390947</v>
+        <v>0.63576906155446367</v>
       </c>
       <c r="AB10" s="23">
         <f t="shared" si="6"/>
-        <v>1.383516686374745</v>
+        <v>1.3773949311252993</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7271,7 +7271,7 @@
         <v>1.0509999999999999</v>
       </c>
       <c r="O11" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P11" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7286,11 +7286,11 @@
       </c>
       <c r="S11" s="23">
         <f t="shared" si="2"/>
-        <v>945.77777777777783</v>
+        <v>941.59292035398244</v>
       </c>
       <c r="T11" s="23">
         <f t="shared" si="3"/>
-        <v>448.28420560915185</v>
+        <v>445.32290604962822</v>
       </c>
       <c r="U11" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B11</f>
@@ -7302,22 +7302,22 @@
       </c>
       <c r="W11">
         <f t="shared" si="4"/>
-        <v>-1.3451512401674819E-2</v>
+        <v>-1.2196055174536192E-2</v>
       </c>
       <c r="X11" s="23">
         <v>2.3297919246001962E-2</v>
       </c>
       <c r="Y11" s="23">
         <f t="shared" si="7"/>
-        <v>945.77777777777783</v>
+        <v>941.59292035398244</v>
       </c>
       <c r="AA11" s="23">
         <f t="shared" si="8"/>
-        <v>0.10123192574122422</v>
+        <v>9.6586932515963717E-2</v>
       </c>
       <c r="AB11" s="23">
         <f t="shared" si="6"/>
-        <v>1.0497684689088878</v>
+        <v>1.0451234756836272</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7368,7 +7368,7 @@
         <v>0.94069999999999998</v>
       </c>
       <c r="O12" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P12" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7383,11 +7383,11 @@
       </c>
       <c r="S12" s="23">
         <f t="shared" si="2"/>
-        <v>925.77777777777771</v>
+        <v>921.68141592920347</v>
       </c>
       <c r="T12" s="23">
         <f t="shared" si="3"/>
-        <v>438.41391355220361</v>
+        <v>435.51610921147039</v>
       </c>
       <c r="U12" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B12</f>
@@ -7399,22 +7399,22 @@
       </c>
       <c r="W12">
         <f t="shared" si="4"/>
-        <v>-7.4515124016747694E-3</v>
+        <v>-6.2226038471024838E-3</v>
       </c>
       <c r="X12" s="23">
         <v>2.3297917690924E-2</v>
       </c>
       <c r="Y12" s="23">
         <f t="shared" si="7"/>
-        <v>925.77777777777771</v>
+        <v>921.68141592920347</v>
       </c>
       <c r="AA12" s="23">
         <f t="shared" si="8"/>
-        <v>7.8327010723698187E-2</v>
+        <v>7.3780243389009334E-2</v>
       </c>
       <c r="AB12" s="23">
         <f t="shared" si="6"/>
-        <v>1.0275694176396677</v>
+        <v>1.0230226503049789</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7465,7 +7465,7 @@
         <v>1.032</v>
       </c>
       <c r="O13" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P13" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7480,11 +7480,11 @@
       </c>
       <c r="S13" s="23">
         <f t="shared" si="2"/>
-        <v>953.33333333333337</v>
+        <v>949.11504424778764</v>
       </c>
       <c r="T13" s="23">
         <f t="shared" si="3"/>
-        <v>451.74017223385897</v>
+        <v>448.75549602666945</v>
       </c>
       <c r="U13" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B13</f>
@@ -7496,22 +7496,22 @@
       </c>
       <c r="W13">
         <f t="shared" si="4"/>
-        <v>-1.5718179068341484E-2</v>
+        <v>-1.4452692342677764E-2</v>
       </c>
       <c r="X13" s="23">
         <v>2.3297920113197729E-2</v>
       </c>
       <c r="Y13" s="23">
         <f t="shared" si="7"/>
-        <v>953.33333333333337</v>
+        <v>949.11504424778764</v>
       </c>
       <c r="AA13" s="23">
         <f t="shared" si="8"/>
-        <v>0.11000767606651593</v>
+        <v>0.10532557528259491</v>
       </c>
       <c r="AB13" s="23">
         <f t="shared" si="6"/>
-        <v>1.0581547771661486</v>
+        <v>1.0534726763822275</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7562,7 +7562,7 @@
         <v>1.6040000000000001</v>
       </c>
       <c r="O14" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P14" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7577,11 +7577,11 @@
       </c>
       <c r="S14" s="23">
         <f t="shared" si="2"/>
-        <v>1724.8888888888891</v>
+        <v>1717.2566371681419</v>
       </c>
       <c r="T14" s="23">
         <f t="shared" si="3"/>
-        <v>816.23950114982279</v>
+        <v>810.84172384303918</v>
       </c>
       <c r="U14" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B14</f>
@@ -7593,22 +7593,22 @@
       </c>
       <c r="W14">
         <f t="shared" si="4"/>
-        <v>2.2413582476216335E-2</v>
+        <v>2.4703257992440511E-2</v>
       </c>
       <c r="X14" s="23">
         <v>2.3297925795726985E-2</v>
       </c>
       <c r="Y14" s="23">
         <f t="shared" si="7"/>
-        <v>1724.8888888888891</v>
+        <v>1717.2566371681419</v>
       </c>
       <c r="AA14" s="23">
         <f t="shared" si="8"/>
-        <v>-1.4313655145940326E-2</v>
+        <v>-1.8554735496368557E-2</v>
       </c>
       <c r="AB14" s="23">
         <f t="shared" si="6"/>
-        <v>0.95848415919678431</v>
+        <v>0.95424307884635617</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7659,7 +7659,7 @@
         <v>1.5049999999999999</v>
       </c>
       <c r="O15" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P15" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7674,11 +7674,11 @@
       </c>
       <c r="S15" s="23">
         <f t="shared" si="2"/>
-        <v>1726.2222222222224</v>
+        <v>1718.5840707964605</v>
       </c>
       <c r="T15" s="23">
         <f t="shared" si="3"/>
-        <v>816.49341237723308</v>
+        <v>811.09230368271699</v>
       </c>
       <c r="U15" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B15</f>
@@ -7690,22 +7690,22 @@
       </c>
       <c r="W15">
         <f t="shared" si="4"/>
-        <v>2.2013582476216341E-2</v>
+        <v>2.4305027903944919E-2</v>
       </c>
       <c r="X15" s="23">
         <v>2.329792734453592E-2</v>
       </c>
       <c r="Y15" s="23">
         <f t="shared" si="7"/>
-        <v>1726.2222222222224</v>
+        <v>1718.5840707964605</v>
       </c>
       <c r="AA15" s="23">
         <f t="shared" si="8"/>
-        <v>-1.3243742417651137E-2</v>
+        <v>-1.7488101108984053E-2</v>
       </c>
       <c r="AB15" s="23">
         <f t="shared" si="6"/>
-        <v>0.95922506424125498</v>
+        <v>0.95498070554992198</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -7756,7 +7756,7 @@
         <v>1.591</v>
       </c>
       <c r="O16" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P16" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7771,11 +7771,11 @@
       </c>
       <c r="S16" s="23">
         <f t="shared" si="2"/>
-        <v>1796.8888888888889</v>
+        <v>1788.9380530973453</v>
       </c>
       <c r="T16" s="23">
         <f t="shared" si="3"/>
-        <v>850.00783716228841</v>
+        <v>844.3854227635843</v>
       </c>
       <c r="U16" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B16</f>
@@ -7787,23 +7787,23 @@
       </c>
       <c r="W16">
         <f t="shared" si="4"/>
-        <v>8.1358247621636797E-4</v>
+        <v>3.1988332136794638E-3</v>
       </c>
       <c r="X16" s="23">
         <v>2.3297930026256426E-2</v>
       </c>
       <c r="Y16" s="23">
         <f t="shared" si="7"/>
-        <v>1796.8888888888889</v>
+        <v>1788.9380530973453</v>
       </c>
       <c r="Z16" s="23"/>
       <c r="AA16" s="23">
         <f t="shared" si="8"/>
-        <v>2.6584756548759001E-2</v>
+        <v>2.2166645789475005E-2</v>
       </c>
       <c r="AB16" s="23">
         <f>Y16*E16/U16</f>
-        <v>0.99849303159819602</v>
+        <v>0.99407492083891202</v>
       </c>
     </row>
     <row r="17" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -7854,7 +7854,7 @@
         <v>6.4370000000000003</v>
       </c>
       <c r="O17" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P17" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7869,11 +7869,11 @@
       </c>
       <c r="S17" s="23">
         <f t="shared" si="2"/>
-        <v>8542.2222222222226</v>
+        <v>8504.424778761062</v>
       </c>
       <c r="T17" s="23">
         <f t="shared" si="3"/>
-        <v>4036.9920410948084</v>
+        <v>4010.2722624893695</v>
       </c>
       <c r="U17" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B17</f>
@@ -7892,18 +7892,18 @@
       </c>
       <c r="Y17" s="23">
         <f>S17</f>
-        <v>8542.2222222222226</v>
+        <v>8504.424778761062</v>
       </c>
       <c r="Z17" s="23">
         <v>750.18565608355891</v>
       </c>
       <c r="AA17" s="23">
         <f t="shared" si="8"/>
-        <v>-3.9811270128704064E-2</v>
+        <v>-4.4001309912319209E-2</v>
       </c>
       <c r="AB17" s="23">
         <f t="shared" si="6"/>
-        <v>0.94694899109701325</v>
+        <v>0.94275895131339815</v>
       </c>
       <c r="AC17" s="23">
         <f>(U17-Q17*G17)/U17</f>
@@ -7958,7 +7958,7 @@
         <v>6.2560000000000002</v>
       </c>
       <c r="O18" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P18" s="1">
         <v>5.0000000000000001E-3</v>
@@ -7973,11 +7973,11 @@
       </c>
       <c r="S18" s="23">
         <f t="shared" si="2"/>
-        <v>8057.7777777777783</v>
+        <v>8022.1238938053111</v>
       </c>
       <c r="T18" s="23">
         <f t="shared" si="3"/>
-        <v>3808.6355656860251</v>
+        <v>3783.4298026536753</v>
       </c>
       <c r="U18" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B18</f>
@@ -7996,18 +7996,18 @@
       </c>
       <c r="Y18" s="23">
         <f t="shared" si="7"/>
-        <v>8057.7777777777783</v>
+        <v>8022.1238938053111</v>
       </c>
       <c r="Z18" s="23">
         <v>696.13408835057783</v>
       </c>
       <c r="AA18" s="23">
         <f t="shared" si="8"/>
-        <v>-9.5721705930232437E-2</v>
+        <v>-9.967412118917833E-2</v>
       </c>
       <c r="AB18" s="23">
         <f t="shared" si="6"/>
-        <v>0.89324584852179245</v>
+        <v>0.8892934332628466</v>
       </c>
       <c r="AC18" s="23">
         <f>(U18-Q18*G18)/U18</f>
@@ -8062,7 +8062,7 @@
         <v>10.15</v>
       </c>
       <c r="O19" s="1">
-        <v>2.2499999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="P19" s="1">
         <v>5.0000000000000001E-3</v>
@@ -8077,11 +8077,11 @@
       </c>
       <c r="S19" s="23">
         <f t="shared" si="2"/>
-        <v>8768.8888888888905</v>
+        <v>8730.0884955752226</v>
       </c>
       <c r="T19" s="23">
         <f t="shared" si="3"/>
-        <v>4158.2359481244393</v>
+        <v>4130.775620894522</v>
       </c>
       <c r="U19" s="23">
         <f>Parameters!$B$6*'Bottle Results'!B19</f>
@@ -8100,15 +8100,15 @@
       </c>
       <c r="Y19" s="23">
         <f t="shared" si="7"/>
-        <v>8768.8888888888905</v>
+        <v>8730.0884955752226</v>
       </c>
       <c r="AA19" s="23">
         <f t="shared" si="8"/>
-        <v>-1.695217839429896E-2</v>
+        <v>-2.1253400294961148E-2</v>
       </c>
       <c r="AB19" s="23">
         <f t="shared" si="6"/>
-        <v>0.97207614954963972</v>
+        <v>0.96777492764897755</v>
       </c>
       <c r="AC19" s="23">
         <f>(U19-Q19*G19)/U19</f>
@@ -8187,7 +8187,7 @@
         <v>1.9506029550982833E-2</v>
       </c>
       <c r="W20" s="28">
-        <f t="shared" ref="W3:W23" si="9">Q20</f>
+        <f t="shared" ref="W20:W23" si="9">Q20</f>
         <v>0</v>
       </c>
       <c r="X20" s="28">
@@ -8455,7 +8455,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8575,11 +8575,11 @@
       </c>
       <c r="D5">
         <f>'Bottle Results'!W5</f>
-        <v>1.3482021684446651E-2</v>
+        <v>-9.7739314566531559E-3</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>0.13482021684446652</v>
+        <v>-9.7739314566531565E-2</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" si="3"/>
@@ -8600,11 +8600,11 @@
       </c>
       <c r="D6">
         <f>'Bottle Results'!W6</f>
-        <v>1.3916215518537662E-2</v>
+        <v>-1.5747382784086782E-2</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>0.13916215518537661</v>
+        <v>-0.15747382784086783</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" si="3"/>
@@ -8625,15 +8625,15 @@
       </c>
       <c r="D7">
         <f>'Bottle Results'!W7</f>
-        <v>1.3087300017091259E-2</v>
+        <v>2.7062351729187552E-2</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>0.13087300017091258</v>
+        <v>0.2706235172918755</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8650,11 +8650,11 @@
       </c>
       <c r="D8">
         <f>'Bottle Results'!W8</f>
-        <v>-2.750530841904502E-2</v>
+        <v>-2.7144718448543558E-2</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>-0.27505308419045021</v>
+        <v>-0.27144718448543559</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" si="3"/>
@@ -8675,11 +8675,11 @@
       </c>
       <c r="D9">
         <f>'Bottle Results'!W9</f>
-        <v>-2.5985308419045026E-2</v>
+        <v>-2.5631444112260374E-2</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>-0.25985308419045028</v>
+        <v>-0.25631444112260376</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" si="3"/>
@@ -8700,11 +8700,11 @@
       </c>
       <c r="D10">
         <f>'Bottle Results'!W10</f>
-        <v>-2.0705308419045023E-2</v>
+        <v>-2.0374806944118778E-2</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>-0.20705308419045024</v>
+        <v>-0.20374806944118778</v>
       </c>
       <c r="F10" t="b">
         <f t="shared" si="3"/>
@@ -8725,11 +8725,11 @@
       </c>
       <c r="D11">
         <f>'Bottle Results'!W11</f>
-        <v>-1.3451512401674819E-2</v>
+        <v>-1.2196055174536192E-2</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>-0.1345151240167482</v>
+        <v>-0.12196055174536191</v>
       </c>
       <c r="F11" t="b">
         <f t="shared" si="3"/>
@@ -8750,11 +8750,11 @@
       </c>
       <c r="D12">
         <f>'Bottle Results'!W12</f>
-        <v>-7.4515124016747694E-3</v>
+        <v>-6.2226038471024838E-3</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>-7.4515124016747689E-2</v>
+        <v>-6.2226038471024842E-2</v>
       </c>
       <c r="F12" t="b">
         <f t="shared" si="3"/>
@@ -8775,11 +8775,11 @@
       </c>
       <c r="D13">
         <f>'Bottle Results'!W13</f>
-        <v>-1.5718179068341484E-2</v>
+        <v>-1.4452692342677764E-2</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>-0.15718179068341484</v>
+        <v>-0.14452692342677764</v>
       </c>
       <c r="F13" t="b">
         <f t="shared" si="3"/>
@@ -8800,11 +8800,11 @@
       </c>
       <c r="D14">
         <f>'Bottle Results'!W14</f>
-        <v>2.2413582476216335E-2</v>
+        <v>2.4703257992440511E-2</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0.22413582476216334</v>
+        <v>0.24703257992440511</v>
       </c>
       <c r="F14" t="b">
         <f t="shared" si="3"/>
@@ -8825,11 +8825,11 @@
       </c>
       <c r="D15">
         <f>'Bottle Results'!W15</f>
-        <v>2.2013582476216341E-2</v>
+        <v>2.4305027903944919E-2</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>0.22013582476216342</v>
+        <v>0.2430502790394492</v>
       </c>
       <c r="F15" t="b">
         <f t="shared" si="3"/>
@@ -8850,11 +8850,11 @@
       </c>
       <c r="D16">
         <f>'Bottle Results'!W16</f>
-        <v>8.1358247621636797E-4</v>
+        <v>3.1988332136794638E-3</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>8.1358247621636792E-3</v>
+        <v>3.1988332136794639E-2</v>
       </c>
       <c r="F16" t="b">
         <f t="shared" si="3"/>
@@ -8945,8 +8945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9035,19 +9035,19 @@
       </c>
       <c r="B3">
         <f>AVERAGE('Bottle Results'!W5:W7)</f>
-        <v>1.3495179073358524E-2</v>
+        <v>5.1367916281587142E-4</v>
       </c>
       <c r="C3">
         <f>_xlfn.STDEV.S('Bottle Results'!W5:W7)</f>
-        <v>4.1461435671810639E-4</v>
+        <v>2.3185006824834382E-2</v>
       </c>
       <c r="D3">
         <f>AVERAGE('Bottle Results'!Y5:Y7)</f>
-        <v>45.223908852763429</v>
+        <v>88.495575221238937</v>
       </c>
       <c r="E3">
         <f>_xlfn.STDEV.S('Bottle Results'!Y5:Y7)</f>
-        <v>1.3820478557270199</v>
+        <v>77.283356082781296</v>
       </c>
       <c r="F3">
         <f>'Bottle Results'!U6</f>
@@ -9055,11 +9055,11 @@
       </c>
       <c r="G3">
         <f>AVERAGE('Bottle Results'!AB5:AB7)</f>
-        <v>0.50133014276052101</v>
+        <v>0.98101867982663704</v>
       </c>
       <c r="H3">
         <f>_xlfn.STDEV.S('Bottle Results'!AB5:AB7)</f>
-        <v>1.532070682057291E-2</v>
+        <v>0.85672550031299244</v>
       </c>
       <c r="I3">
         <f>AVERAGE('Bottle Results'!D5:D7)</f>
@@ -9076,19 +9076,19 @@
       </c>
       <c r="B4">
         <f>AVERAGE('Bottle Results'!W8:W10)</f>
-        <v>-2.4731975085711691E-2</v>
+        <v>-2.4383656501640903E-2</v>
       </c>
       <c r="C4">
         <f>_xlfn.STDEV.S('Bottle Results'!W8:W10)</f>
-        <v>3.5690521617557413E-3</v>
+        <v>3.5532598955532839E-3</v>
       </c>
       <c r="D4">
         <f>AVERAGE('Bottle Results'!Y8:Y10)</f>
-        <v>262.39999999999998</v>
+        <v>261.2389380530974</v>
       </c>
       <c r="E4">
         <f>_xlfn.STDEV.S('Bottle Results'!Y8:Y10)</f>
-        <v>11.896840539185801</v>
+        <v>11.844199651844281</v>
       </c>
       <c r="F4">
         <f>'Bottle Results'!U9</f>
@@ -9096,11 +9096,11 @@
       </c>
       <c r="G4">
         <f>AVERAGE('Bottle Results'!AB8:AB10)</f>
-        <v>1.4581011275181173</v>
+        <v>1.4516493526175951</v>
       </c>
       <c r="H4">
         <f>_xlfn.STDEV.S('Bottle Results'!AB8:AB10)</f>
-        <v>6.6108218765587104E-2</v>
+        <v>6.5815704523261576E-2</v>
       </c>
       <c r="I4">
         <f>AVERAGE('Bottle Results'!D8:D10)</f>
@@ -9117,19 +9117,19 @@
       </c>
       <c r="B5">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
-        <v>-1.2207067957230358E-2</v>
+        <v>-1.0957117121438813E-2</v>
       </c>
       <c r="C5">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
-        <v>4.2715250117406709E-3</v>
+        <v>4.2526244585913853E-3</v>
       </c>
       <c r="D5">
         <f>AVERAGE('Bottle Results'!Y11:Y13)</f>
-        <v>941.62962962962968</v>
+        <v>937.46312684365785</v>
       </c>
       <c r="E5">
         <f>_xlfn.STDEV.S('Bottle Results'!Y11:Y13)</f>
-        <v>14.23841670580221</v>
+        <v>14.175414861971241</v>
       </c>
       <c r="F5">
         <f>'Bottle Results'!U12</f>
@@ -9137,11 +9137,11 @@
       </c>
       <c r="G5">
         <f>AVERAGE('Bottle Results'!AB11:AB13)</f>
-        <v>1.0451642212382346</v>
+        <v>1.0405396007902779</v>
       </c>
       <c r="H5">
         <f>_xlfn.STDEV.S('Bottle Results'!AB11:AB13)</f>
-        <v>1.580396712223104E-2</v>
+        <v>1.5734038064168072E-2</v>
       </c>
       <c r="I5">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
@@ -9158,19 +9158,19 @@
       </c>
       <c r="B6">
         <f>AVERAGE('Bottle Results'!W14:W16)</f>
-        <v>1.5080249142883015E-2</v>
+        <v>1.7402373036688297E-2</v>
       </c>
       <c r="C6">
         <f>_xlfn.STDEV.S('Bottle Results'!W14:W16)</f>
-        <v>1.2356914393704153E-2</v>
+        <v>1.2302237781342635E-2</v>
       </c>
       <c r="D6">
         <f>AVERAGE('Bottle Results'!Y14:Y16)</f>
-        <v>1749.3333333333333</v>
+        <v>1741.5929203539824</v>
       </c>
       <c r="E6">
         <f>_xlfn.STDEV.S('Bottle Results'!Y14:Y16)</f>
-        <v>41.189714645680461</v>
+        <v>41.007459271142103</v>
       </c>
       <c r="F6">
         <f>'Bottle Results'!U15</f>
@@ -9178,11 +9178,11 @@
       </c>
       <c r="G6">
         <f>AVERAGE('Bottle Results'!AB14:AB16)</f>
-        <v>0.97206741834541177</v>
+        <v>0.96776623507839676</v>
       </c>
       <c r="H6">
         <f>_xlfn.STDEV.S('Bottle Results'!AB14:AB16)</f>
-        <v>2.288825052096655E-2</v>
+        <v>2.2786975076183512E-2</v>
       </c>
       <c r="I6">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
@@ -9207,11 +9207,11 @@
       </c>
       <c r="D7">
         <f>AVERAGE('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>8548.0966523683819</v>
+        <v>8520.0337221815589</v>
       </c>
       <c r="E7">
         <f>_xlfn.STDEV.S('Bottle Results'!Y17:Y19,'Bottle Results'!Y21)</f>
-        <v>348.8275924635368</v>
+        <v>357.94377699140438</v>
       </c>
       <c r="F7">
         <f>'Bottle Results'!U18</f>
@@ -9219,11 +9219,11 @@
       </c>
       <c r="G7">
         <f>AVERAGE('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>0.94760020170187265</v>
+        <v>0.94448928246606678</v>
       </c>
       <c r="H7">
         <f>_xlfn.STDEV.S('Bottle Results'!AB17:AB19,'Bottle Results'!AB21)</f>
-        <v>3.8669321419762176E-2</v>
+        <v>3.9679897065858227E-2</v>
       </c>
       <c r="I7">
         <f>AVERAGE('Bottle Results'!D17:D19,'Bottle Results'!D21)</f>

</xml_diff>